<commit_message>
fix legend text typo in demo_sample.xlsx
</commit_message>
<xml_diff>
--- a/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
+++ b/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
@@ -4,15 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="22995" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="22995" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Liquidity" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -1028,36 +1025,11 @@
     <xf numFmtId="165" fontId="11" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1080,7 +1052,6 @@
     <xf numFmtId="165" fontId="3" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1122,6 +1093,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1151,7 +1148,7 @@
             <c:strLit>
               <c:ptCount val="3"/>
               <c:pt idx="0">
-                <c:v>asserts</c:v>
+                <c:v>assets</c:v>
               </c:pt>
               <c:pt idx="1">
                 <c:v>liabilities</c:v>
@@ -1195,7 +1192,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.7330779054916986"/>
-          <c:y val="0.30801248699271655"/>
+          <c:y val="0.30801248699271666"/>
           <c:w val="0.23499361430395913"/>
           <c:h val="0.37044745057232054"/>
         </c:manualLayout>
@@ -1216,7 +1213,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1257,45 +1254,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Input"/>
-      <sheetName val="Liquidity"/>
-      <sheetName val="Assets"/>
-      <sheetName val="Profitability"/>
-      <sheetName val="Debt"/>
-      <sheetName val="Market"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="15">
-          <cell r="J15">
-            <v>136000</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="J21">
-            <v>110000</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="J22">
-            <v>26000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1585,7 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:J4"/>
     </sheetView>
   </sheetViews>
@@ -1636,17 +1594,17 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="2:10" ht="29.25" customHeight="1">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="129"/>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="52"/>
@@ -1660,12 +1618,12 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="30">
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
       <c r="F6" s="53" t="s">
         <v>36</v>
       </c>
@@ -1746,12 +1704,12 @@
       <c r="J11" s="52"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="102"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="102"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="69" t="s">
         <v>2</v>
       </c>
@@ -2481,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AJ58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
@@ -2582,58 +2540,58 @@
       <c r="AJ2" s="3"/>
     </row>
     <row r="3" spans="2:36">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="108" t="s">
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="109"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
-      <c r="M3" s="108" t="s">
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109" t="s">
+      <c r="N3" s="135"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="108" t="s">
+      <c r="Q3" s="135"/>
+      <c r="R3" s="135"/>
+      <c r="S3" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="109"/>
-      <c r="U3" s="109"/>
-      <c r="V3" s="109"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="109"/>
-      <c r="Y3" s="108" t="s">
+      <c r="T3" s="135"/>
+      <c r="U3" s="135"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="135"/>
+      <c r="X3" s="135"/>
+      <c r="Y3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="109"/>
-      <c r="AA3" s="109"/>
-      <c r="AB3" s="109"/>
-      <c r="AC3" s="109"/>
-      <c r="AD3" s="109"/>
-      <c r="AE3" s="108" t="s">
+      <c r="Z3" s="135"/>
+      <c r="AA3" s="135"/>
+      <c r="AB3" s="135"/>
+      <c r="AC3" s="135"/>
+      <c r="AD3" s="135"/>
+      <c r="AE3" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="109"/>
-      <c r="AG3" s="109"/>
-      <c r="AH3" s="109"/>
-      <c r="AI3" s="109"/>
-      <c r="AJ3" s="110"/>
+      <c r="AF3" s="135"/>
+      <c r="AG3" s="135"/>
+      <c r="AH3" s="135"/>
+      <c r="AI3" s="135"/>
+      <c r="AJ3" s="136"/>
     </row>
     <row r="4" spans="2:36">
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="102" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="8"/>
@@ -2669,10 +2627,10 @@
       <c r="AG4" s="14"/>
       <c r="AH4" s="14"/>
       <c r="AI4" s="14"/>
-      <c r="AJ4" s="112"/>
+      <c r="AJ4" s="103"/>
     </row>
     <row r="5" spans="2:36">
-      <c r="B5" s="113"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="16"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2706,10 +2664,10 @@
       <c r="AG5" s="2"/>
       <c r="AH5" s="20"/>
       <c r="AI5" s="20"/>
-      <c r="AJ5" s="114"/>
+      <c r="AJ5" s="105"/>
     </row>
     <row r="6" spans="2:36">
-      <c r="B6" s="115"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="16" t="s">
         <v>8</v>
       </c>
@@ -2789,10 +2747,10 @@
         <v>56000</v>
       </c>
       <c r="AI6" s="20"/>
-      <c r="AJ6" s="114"/>
+      <c r="AJ6" s="105"/>
     </row>
     <row r="7" spans="2:36">
-      <c r="B7" s="115"/>
+      <c r="B7" s="106"/>
       <c r="C7" s="16"/>
       <c r="D7" s="2"/>
       <c r="E7" s="27" t="s">
@@ -2843,10 +2801,10 @@
         <v>25600</v>
       </c>
       <c r="AI7" s="20"/>
-      <c r="AJ7" s="114"/>
+      <c r="AJ7" s="105"/>
     </row>
     <row r="8" spans="2:36">
-      <c r="B8" s="115"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
@@ -2892,17 +2850,17 @@
       <c r="AG8" s="2"/>
       <c r="AH8" s="20"/>
       <c r="AI8" s="20"/>
-      <c r="AJ8" s="114"/>
+      <c r="AJ8" s="105"/>
     </row>
     <row r="9" spans="2:36">
-      <c r="B9" s="115"/>
+      <c r="B9" s="106"/>
       <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="137"/>
+      <c r="G9" s="127"/>
       <c r="H9" s="25">
         <f>H6-H8</f>
         <v>-4.3478260869565188E-2</v>
@@ -2946,10 +2904,10 @@
       <c r="AG9" s="32"/>
       <c r="AH9" s="32"/>
       <c r="AI9" s="32"/>
-      <c r="AJ9" s="116"/>
+      <c r="AJ9" s="107"/>
     </row>
     <row r="10" spans="2:36">
-      <c r="B10" s="117"/>
+      <c r="B10" s="108"/>
       <c r="C10" s="35" t="s">
         <v>14</v>
       </c>
@@ -2994,10 +2952,10 @@
       <c r="AG10" s="38"/>
       <c r="AH10" s="38"/>
       <c r="AI10" s="38"/>
-      <c r="AJ10" s="118"/>
+      <c r="AJ10" s="109"/>
     </row>
     <row r="11" spans="2:36">
-      <c r="B11" s="115"/>
+      <c r="B11" s="106"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -3031,10 +2989,10 @@
       <c r="AG11" s="32"/>
       <c r="AH11" s="32"/>
       <c r="AI11" s="32"/>
-      <c r="AJ11" s="116"/>
+      <c r="AJ11" s="107"/>
     </row>
     <row r="12" spans="2:36">
-      <c r="B12" s="115"/>
+      <c r="B12" s="106"/>
       <c r="C12" s="16" t="s">
         <v>15</v>
       </c>
@@ -3136,13 +3094,13 @@
       <c r="AI12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AJ12" s="119">
+      <c r="AJ12" s="110">
         <f>Input!J18</f>
         <v>14350</v>
       </c>
     </row>
     <row r="13" spans="2:36">
-      <c r="B13" s="115"/>
+      <c r="B13" s="106"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
       <c r="E13" s="27" t="s">
@@ -3152,51 +3110,51 @@
       <c r="G13" s="18"/>
       <c r="H13" s="19"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="104">
+      <c r="J13" s="131">
         <f>Input!F20</f>
         <v>23000</v>
       </c>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
+      <c r="K13" s="132"/>
+      <c r="L13" s="132"/>
       <c r="M13" s="48"/>
       <c r="N13" s="19"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="104">
+      <c r="P13" s="131">
         <f>Input!G20</f>
         <v>25000</v>
       </c>
-      <c r="Q13" s="105"/>
-      <c r="R13" s="105"/>
+      <c r="Q13" s="132"/>
+      <c r="R13" s="132"/>
       <c r="S13" s="48"/>
       <c r="T13" s="19"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="104">
+      <c r="V13" s="131">
         <f>Input!H20</f>
         <v>22500</v>
       </c>
-      <c r="W13" s="105"/>
-      <c r="X13" s="105"/>
+      <c r="W13" s="132"/>
+      <c r="X13" s="132"/>
       <c r="Y13" s="48"/>
       <c r="Z13" s="19"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="104">
+      <c r="AB13" s="131">
         <f>Input!I20</f>
         <v>25600</v>
       </c>
-      <c r="AC13" s="105"/>
-      <c r="AD13" s="105"/>
+      <c r="AC13" s="132"/>
+      <c r="AD13" s="132"/>
       <c r="AE13" s="48"/>
       <c r="AF13" s="19"/>
       <c r="AG13" s="2"/>
-      <c r="AH13" s="104">
+      <c r="AH13" s="131">
         <f>Input!J20</f>
         <v>25600</v>
       </c>
-      <c r="AI13" s="105"/>
-      <c r="AJ13" s="120"/>
+      <c r="AI13" s="132"/>
+      <c r="AJ13" s="133"/>
     </row>
     <row r="14" spans="2:36">
-      <c r="B14" s="115"/>
+      <c r="B14" s="106"/>
       <c r="C14" s="16" t="s">
         <v>12</v>
       </c>
@@ -3242,10 +3200,10 @@
       <c r="AG14" s="2"/>
       <c r="AH14" s="20"/>
       <c r="AI14" s="20"/>
-      <c r="AJ14" s="114"/>
+      <c r="AJ14" s="105"/>
     </row>
     <row r="15" spans="2:36">
-      <c r="B15" s="115"/>
+      <c r="B15" s="106"/>
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
@@ -3296,10 +3254,10 @@
       <c r="AG15" s="2"/>
       <c r="AH15" s="20"/>
       <c r="AI15" s="20"/>
-      <c r="AJ15" s="114"/>
+      <c r="AJ15" s="105"/>
     </row>
     <row r="16" spans="2:36">
-      <c r="B16" s="117"/>
+      <c r="B16" s="108"/>
       <c r="C16" s="35" t="s">
         <v>14</v>
       </c>
@@ -3344,10 +3302,10 @@
       <c r="AG16" s="36"/>
       <c r="AH16" s="40"/>
       <c r="AI16" s="40"/>
-      <c r="AJ16" s="121"/>
+      <c r="AJ16" s="111"/>
     </row>
     <row r="17" spans="2:36">
-      <c r="B17" s="115"/>
+      <c r="B17" s="106"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3381,11 +3339,11 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="20"/>
       <c r="AI17" s="20"/>
-      <c r="AJ17" s="114"/>
+      <c r="AJ17" s="105"/>
     </row>
     <row r="18" spans="2:36">
-      <c r="B18" s="115"/>
-      <c r="C18" s="103" t="s">
+      <c r="B18" s="106"/>
+      <c r="C18" s="137" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -3486,14 +3444,14 @@
       <c r="AI18" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AJ18" s="122">
+      <c r="AJ18" s="112">
         <f>Input!J20</f>
         <v>25600</v>
       </c>
     </row>
     <row r="19" spans="2:36">
-      <c r="B19" s="115"/>
-      <c r="C19" s="103"/>
+      <c r="B19" s="106"/>
+      <c r="C19" s="137"/>
       <c r="D19" s="2"/>
       <c r="E19" s="27" t="s">
         <v>20</v>
@@ -3502,51 +3460,51 @@
       <c r="G19" s="18"/>
       <c r="H19" s="19"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="104">
+      <c r="J19" s="131">
         <f>Input!F15</f>
         <v>125000</v>
       </c>
-      <c r="K19" s="105"/>
-      <c r="L19" s="105"/>
+      <c r="K19" s="132"/>
+      <c r="L19" s="132"/>
       <c r="M19" s="48"/>
       <c r="N19" s="19"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="104">
+      <c r="P19" s="131">
         <f>Input!G15</f>
         <v>126000</v>
       </c>
-      <c r="Q19" s="105"/>
-      <c r="R19" s="105"/>
+      <c r="Q19" s="132"/>
+      <c r="R19" s="132"/>
       <c r="S19" s="48"/>
       <c r="T19" s="19"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="104">
+      <c r="V19" s="131">
         <f>Input!H15</f>
         <v>126500</v>
       </c>
-      <c r="W19" s="105"/>
-      <c r="X19" s="105"/>
+      <c r="W19" s="132"/>
+      <c r="X19" s="132"/>
       <c r="Y19" s="48"/>
       <c r="Z19" s="19"/>
       <c r="AA19" s="2"/>
-      <c r="AB19" s="104">
+      <c r="AB19" s="131">
         <f>Input!I15</f>
         <v>136000</v>
       </c>
-      <c r="AC19" s="105"/>
-      <c r="AD19" s="105"/>
+      <c r="AC19" s="132"/>
+      <c r="AD19" s="132"/>
       <c r="AE19" s="48"/>
       <c r="AF19" s="25"/>
       <c r="AG19" s="2"/>
-      <c r="AH19" s="104">
+      <c r="AH19" s="131">
         <f>Input!J15</f>
         <v>136000</v>
       </c>
-      <c r="AI19" s="105"/>
-      <c r="AJ19" s="120"/>
+      <c r="AI19" s="132"/>
+      <c r="AJ19" s="133"/>
     </row>
     <row r="20" spans="2:36">
-      <c r="B20" s="115"/>
+      <c r="B20" s="106"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -3580,10 +3538,10 @@
       <c r="AG20" s="2"/>
       <c r="AH20" s="20"/>
       <c r="AI20" s="20"/>
-      <c r="AJ20" s="114"/>
+      <c r="AJ20" s="105"/>
     </row>
     <row r="21" spans="2:36">
-      <c r="B21" s="115"/>
+      <c r="B21" s="106"/>
       <c r="C21" s="16" t="s">
         <v>12</v>
       </c>
@@ -3629,10 +3587,10 @@
       <c r="AG21" s="2"/>
       <c r="AH21" s="20"/>
       <c r="AI21" s="20"/>
-      <c r="AJ21" s="114"/>
+      <c r="AJ21" s="105"/>
     </row>
     <row r="22" spans="2:36">
-      <c r="B22" s="115"/>
+      <c r="B22" s="106"/>
       <c r="C22" s="16" t="s">
         <v>13</v>
       </c>
@@ -3683,10 +3641,10 @@
       <c r="AG22" s="2"/>
       <c r="AH22" s="20"/>
       <c r="AI22" s="20"/>
-      <c r="AJ22" s="114"/>
+      <c r="AJ22" s="105"/>
     </row>
     <row r="23" spans="2:36">
-      <c r="B23" s="117"/>
+      <c r="B23" s="108"/>
       <c r="C23" s="35" t="s">
         <v>14</v>
       </c>
@@ -3731,10 +3689,10 @@
       <c r="AG23" s="36"/>
       <c r="AH23" s="40"/>
       <c r="AI23" s="40"/>
-      <c r="AJ23" s="121"/>
+      <c r="AJ23" s="111"/>
     </row>
     <row r="24" spans="2:36">
-      <c r="B24" s="115"/>
+      <c r="B24" s="106"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -3768,11 +3726,11 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="20"/>
       <c r="AI24" s="20"/>
-      <c r="AJ24" s="114"/>
+      <c r="AJ24" s="105"/>
     </row>
     <row r="25" spans="2:36">
-      <c r="B25" s="115"/>
-      <c r="C25" s="103" t="s">
+      <c r="B25" s="106"/>
+      <c r="C25" s="137" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -3851,11 +3809,11 @@
         <v>25600</v>
       </c>
       <c r="AI25" s="20"/>
-      <c r="AJ25" s="114"/>
+      <c r="AJ25" s="105"/>
     </row>
     <row r="26" spans="2:36">
-      <c r="B26" s="115"/>
-      <c r="C26" s="103"/>
+      <c r="B26" s="106"/>
+      <c r="C26" s="137"/>
       <c r="D26" s="2"/>
       <c r="E26" s="27" t="s">
         <v>22</v>
@@ -3905,10 +3863,10 @@
         <v>14350</v>
       </c>
       <c r="AI26" s="20"/>
-      <c r="AJ26" s="114"/>
+      <c r="AJ26" s="105"/>
     </row>
     <row r="27" spans="2:36">
-      <c r="B27" s="115"/>
+      <c r="B27" s="106"/>
       <c r="C27" s="49"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -3942,10 +3900,10 @@
       <c r="AG27" s="2"/>
       <c r="AH27" s="20"/>
       <c r="AI27" s="20"/>
-      <c r="AJ27" s="114"/>
+      <c r="AJ27" s="105"/>
     </row>
     <row r="28" spans="2:36">
-      <c r="B28" s="115"/>
+      <c r="B28" s="106"/>
       <c r="C28" s="16" t="s">
         <v>12</v>
       </c>
@@ -3991,10 +3949,10 @@
       <c r="AG28" s="2"/>
       <c r="AH28" s="20"/>
       <c r="AI28" s="20"/>
-      <c r="AJ28" s="114"/>
+      <c r="AJ28" s="105"/>
     </row>
     <row r="29" spans="2:36">
-      <c r="B29" s="115"/>
+      <c r="B29" s="106"/>
       <c r="C29" s="16" t="s">
         <v>13</v>
       </c>
@@ -4045,10 +4003,10 @@
       <c r="AG29" s="2"/>
       <c r="AH29" s="20"/>
       <c r="AI29" s="20"/>
-      <c r="AJ29" s="114"/>
+      <c r="AJ29" s="105"/>
     </row>
     <row r="30" spans="2:36">
-      <c r="B30" s="117"/>
+      <c r="B30" s="108"/>
       <c r="C30" s="35" t="s">
         <v>14</v>
       </c>
@@ -4093,10 +4051,10 @@
       <c r="AG30" s="36"/>
       <c r="AH30" s="40"/>
       <c r="AI30" s="40"/>
-      <c r="AJ30" s="121"/>
+      <c r="AJ30" s="111"/>
     </row>
     <row r="31" spans="2:36">
-      <c r="B31" s="115"/>
+      <c r="B31" s="106"/>
       <c r="C31" s="16"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -4130,10 +4088,10 @@
       <c r="AG31" s="2"/>
       <c r="AH31" s="20"/>
       <c r="AI31" s="20"/>
-      <c r="AJ31" s="114"/>
+      <c r="AJ31" s="105"/>
     </row>
     <row r="32" spans="2:36">
-      <c r="B32" s="115"/>
+      <c r="B32" s="106"/>
       <c r="C32" s="16" t="s">
         <v>23</v>
       </c>
@@ -4213,10 +4171,10 @@
         <v>14350</v>
       </c>
       <c r="AI32" s="20"/>
-      <c r="AJ32" s="114"/>
+      <c r="AJ32" s="105"/>
     </row>
     <row r="33" spans="2:36">
-      <c r="B33" s="115"/>
+      <c r="B33" s="106"/>
       <c r="C33" s="16"/>
       <c r="D33" s="2"/>
       <c r="E33" s="27" t="s">
@@ -4267,10 +4225,10 @@
         <v>25600</v>
       </c>
       <c r="AI33" s="20"/>
-      <c r="AJ33" s="114"/>
+      <c r="AJ33" s="105"/>
     </row>
     <row r="34" spans="2:36">
-      <c r="B34" s="115"/>
+      <c r="B34" s="106"/>
       <c r="C34" s="16" t="s">
         <v>12</v>
       </c>
@@ -4316,10 +4274,10 @@
       <c r="AG34" s="2"/>
       <c r="AH34" s="20"/>
       <c r="AI34" s="20"/>
-      <c r="AJ34" s="114"/>
+      <c r="AJ34" s="105"/>
     </row>
     <row r="35" spans="2:36">
-      <c r="B35" s="115"/>
+      <c r="B35" s="106"/>
       <c r="C35" s="16" t="s">
         <v>13</v>
       </c>
@@ -4370,10 +4328,10 @@
       <c r="AG35" s="2"/>
       <c r="AH35" s="20"/>
       <c r="AI35" s="20"/>
-      <c r="AJ35" s="114"/>
+      <c r="AJ35" s="105"/>
     </row>
     <row r="36" spans="2:36">
-      <c r="B36" s="117"/>
+      <c r="B36" s="108"/>
       <c r="C36" s="35" t="s">
         <v>14</v>
       </c>
@@ -4418,10 +4376,10 @@
       <c r="AG36" s="36"/>
       <c r="AH36" s="40"/>
       <c r="AI36" s="40"/>
-      <c r="AJ36" s="121"/>
+      <c r="AJ36" s="111"/>
     </row>
     <row r="37" spans="2:36">
-      <c r="B37" s="115"/>
+      <c r="B37" s="106"/>
       <c r="C37" s="16"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -4455,10 +4413,10 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="20"/>
       <c r="AI37" s="20"/>
-      <c r="AJ37" s="114"/>
+      <c r="AJ37" s="105"/>
     </row>
     <row r="38" spans="2:36">
-      <c r="B38" s="115"/>
+      <c r="B38" s="106"/>
       <c r="C38" s="16" t="s">
         <v>25</v>
       </c>
@@ -4538,10 +4496,10 @@
         <v>272000</v>
       </c>
       <c r="AI38" s="20"/>
-      <c r="AJ38" s="114"/>
+      <c r="AJ38" s="105"/>
     </row>
     <row r="39" spans="2:36">
-      <c r="B39" s="115"/>
+      <c r="B39" s="106"/>
       <c r="C39" s="16"/>
       <c r="D39" s="2"/>
       <c r="E39" s="27" t="s">
@@ -4592,10 +4550,10 @@
         <v>289600</v>
       </c>
       <c r="AI39" s="20"/>
-      <c r="AJ39" s="114"/>
+      <c r="AJ39" s="105"/>
     </row>
     <row r="40" spans="2:36">
-      <c r="B40" s="115"/>
+      <c r="B40" s="106"/>
       <c r="C40" s="16" t="s">
         <v>12</v>
       </c>
@@ -4641,10 +4599,10 @@
       <c r="AG40" s="2"/>
       <c r="AH40" s="20"/>
       <c r="AI40" s="20"/>
-      <c r="AJ40" s="114"/>
+      <c r="AJ40" s="105"/>
     </row>
     <row r="41" spans="2:36">
-      <c r="B41" s="115"/>
+      <c r="B41" s="106"/>
       <c r="C41" s="16" t="s">
         <v>13</v>
       </c>
@@ -4695,10 +4653,10 @@
       <c r="AG41" s="2"/>
       <c r="AH41" s="20"/>
       <c r="AI41" s="20"/>
-      <c r="AJ41" s="114"/>
+      <c r="AJ41" s="105"/>
     </row>
     <row r="42" spans="2:36">
-      <c r="B42" s="117"/>
+      <c r="B42" s="108"/>
       <c r="C42" s="35" t="s">
         <v>14</v>
       </c>
@@ -4743,10 +4701,10 @@
       <c r="AG42" s="36"/>
       <c r="AH42" s="40"/>
       <c r="AI42" s="40"/>
-      <c r="AJ42" s="121"/>
+      <c r="AJ42" s="111"/>
     </row>
     <row r="43" spans="2:36">
-      <c r="B43" s="115"/>
+      <c r="B43" s="106"/>
       <c r="C43" s="16"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -4780,10 +4738,10 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="20"/>
       <c r="AI43" s="20"/>
-      <c r="AJ43" s="114"/>
+      <c r="AJ43" s="105"/>
     </row>
     <row r="44" spans="2:36">
-      <c r="B44" s="123" t="s">
+      <c r="B44" s="113" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="2"/>
@@ -4819,10 +4777,10 @@
       <c r="AG44" s="2"/>
       <c r="AH44" s="20"/>
       <c r="AI44" s="20"/>
-      <c r="AJ44" s="114"/>
+      <c r="AJ44" s="105"/>
     </row>
     <row r="45" spans="2:36">
-      <c r="B45" s="115"/>
+      <c r="B45" s="106"/>
       <c r="C45" s="16"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -4856,11 +4814,11 @@
       <c r="AG45" s="2"/>
       <c r="AH45" s="20"/>
       <c r="AI45" s="20"/>
-      <c r="AJ45" s="124"/>
+      <c r="AJ45" s="114"/>
     </row>
     <row r="46" spans="2:36">
-      <c r="B46" s="115"/>
-      <c r="C46" s="103" t="s">
+      <c r="B46" s="106"/>
+      <c r="C46" s="137" t="s">
         <v>29</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -4939,11 +4897,11 @@
         <v>72000</v>
       </c>
       <c r="AI46" s="20"/>
-      <c r="AJ46" s="124"/>
+      <c r="AJ46" s="114"/>
     </row>
     <row r="47" spans="2:36">
-      <c r="B47" s="115"/>
-      <c r="C47" s="103"/>
+      <c r="B47" s="106"/>
+      <c r="C47" s="137"/>
       <c r="D47" s="2"/>
       <c r="E47" s="27" t="s">
         <v>31</v>
@@ -4993,10 +4951,10 @@
         <v>561600</v>
       </c>
       <c r="AI47" s="20"/>
-      <c r="AJ47" s="124"/>
+      <c r="AJ47" s="114"/>
     </row>
     <row r="48" spans="2:36">
-      <c r="B48" s="115"/>
+      <c r="B48" s="106"/>
       <c r="C48" s="49"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -5030,10 +4988,10 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="20"/>
       <c r="AI48" s="20"/>
-      <c r="AJ48" s="124"/>
+      <c r="AJ48" s="114"/>
     </row>
     <row r="49" spans="2:36">
-      <c r="B49" s="115"/>
+      <c r="B49" s="106"/>
       <c r="C49" s="16" t="s">
         <v>12</v>
       </c>
@@ -5079,10 +5037,10 @@
       <c r="AG49" s="2"/>
       <c r="AH49" s="20"/>
       <c r="AI49" s="20"/>
-      <c r="AJ49" s="124"/>
+      <c r="AJ49" s="114"/>
     </row>
     <row r="50" spans="2:36">
-      <c r="B50" s="115"/>
+      <c r="B50" s="106"/>
       <c r="C50" s="16" t="s">
         <v>13</v>
       </c>
@@ -5133,10 +5091,10 @@
       <c r="AG50" s="2"/>
       <c r="AH50" s="20"/>
       <c r="AI50" s="20"/>
-      <c r="AJ50" s="124"/>
+      <c r="AJ50" s="114"/>
     </row>
     <row r="51" spans="2:36">
-      <c r="B51" s="117"/>
+      <c r="B51" s="108"/>
       <c r="C51" s="35" t="s">
         <v>14</v>
       </c>
@@ -5181,10 +5139,10 @@
       <c r="AG51" s="36"/>
       <c r="AH51" s="40"/>
       <c r="AI51" s="40"/>
-      <c r="AJ51" s="125"/>
+      <c r="AJ51" s="115"/>
     </row>
     <row r="52" spans="2:36">
-      <c r="B52" s="115"/>
+      <c r="B52" s="106"/>
       <c r="C52" s="16"/>
       <c r="D52" s="32"/>
       <c r="E52" s="32"/>
@@ -5218,10 +5176,10 @@
       <c r="AG52" s="2"/>
       <c r="AH52" s="20"/>
       <c r="AI52" s="20"/>
-      <c r="AJ52" s="124"/>
+      <c r="AJ52" s="114"/>
     </row>
     <row r="53" spans="2:36">
-      <c r="B53" s="115"/>
+      <c r="B53" s="106"/>
       <c r="C53" s="16" t="s">
         <v>32</v>
       </c>
@@ -5301,10 +5259,10 @@
         <v>44000</v>
       </c>
       <c r="AI53" s="20"/>
-      <c r="AJ53" s="124"/>
+      <c r="AJ53" s="114"/>
     </row>
     <row r="54" spans="2:36">
-      <c r="B54" s="115"/>
+      <c r="B54" s="106"/>
       <c r="C54" s="16" t="s">
         <v>33</v>
       </c>
@@ -5357,10 +5315,10 @@
         <v>561600</v>
       </c>
       <c r="AI54" s="20"/>
-      <c r="AJ54" s="124"/>
+      <c r="AJ54" s="114"/>
     </row>
     <row r="55" spans="2:36">
-      <c r="B55" s="115"/>
+      <c r="B55" s="106"/>
       <c r="C55" s="16"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -5394,10 +5352,10 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="20"/>
       <c r="AI55" s="20"/>
-      <c r="AJ55" s="124"/>
+      <c r="AJ55" s="114"/>
     </row>
     <row r="56" spans="2:36">
-      <c r="B56" s="115"/>
+      <c r="B56" s="106"/>
       <c r="C56" s="16" t="s">
         <v>12</v>
       </c>
@@ -5443,10 +5401,10 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="20"/>
       <c r="AI56" s="20"/>
-      <c r="AJ56" s="124"/>
+      <c r="AJ56" s="114"/>
     </row>
     <row r="57" spans="2:36">
-      <c r="B57" s="115"/>
+      <c r="B57" s="106"/>
       <c r="C57" s="16" t="s">
         <v>13</v>
       </c>
@@ -5497,58 +5455,63 @@
       <c r="AG57" s="32"/>
       <c r="AH57" s="32"/>
       <c r="AI57" s="32"/>
-      <c r="AJ57" s="116"/>
+      <c r="AJ57" s="107"/>
     </row>
     <row r="58" spans="2:36">
-      <c r="B58" s="126"/>
-      <c r="C58" s="127" t="s">
+      <c r="B58" s="116"/>
+      <c r="C58" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="128"/>
-      <c r="E58" s="128"/>
-      <c r="F58" s="129"/>
-      <c r="G58" s="130"/>
-      <c r="H58" s="131"/>
-      <c r="I58" s="128"/>
-      <c r="J58" s="132"/>
-      <c r="K58" s="132"/>
-      <c r="L58" s="128"/>
-      <c r="M58" s="133"/>
-      <c r="N58" s="134">
+      <c r="D58" s="118"/>
+      <c r="E58" s="118"/>
+      <c r="F58" s="119"/>
+      <c r="G58" s="120"/>
+      <c r="H58" s="121"/>
+      <c r="I58" s="118"/>
+      <c r="J58" s="122"/>
+      <c r="K58" s="122"/>
+      <c r="L58" s="118"/>
+      <c r="M58" s="123"/>
+      <c r="N58" s="124">
         <f>N53-H53</f>
         <v>-5.3492484526967282E-3</v>
       </c>
-      <c r="O58" s="128"/>
-      <c r="P58" s="128"/>
-      <c r="Q58" s="128"/>
-      <c r="R58" s="130"/>
-      <c r="S58" s="135"/>
-      <c r="T58" s="134">
+      <c r="O58" s="118"/>
+      <c r="P58" s="118"/>
+      <c r="Q58" s="118"/>
+      <c r="R58" s="120"/>
+      <c r="S58" s="125"/>
+      <c r="T58" s="124">
         <f>T53-N53</f>
         <v>1.0608123439981854E-2</v>
       </c>
-      <c r="U58" s="130"/>
-      <c r="V58" s="130"/>
-      <c r="W58" s="130"/>
-      <c r="X58" s="130"/>
-      <c r="Y58" s="135"/>
-      <c r="Z58" s="134">
+      <c r="U58" s="120"/>
+      <c r="V58" s="120"/>
+      <c r="W58" s="120"/>
+      <c r="X58" s="120"/>
+      <c r="Y58" s="125"/>
+      <c r="Z58" s="124">
         <f>Z53-T53</f>
         <v>6.8790560471976292E-3</v>
       </c>
-      <c r="AA58" s="130"/>
-      <c r="AB58" s="130"/>
-      <c r="AC58" s="130"/>
-      <c r="AD58" s="130"/>
-      <c r="AE58" s="135"/>
-      <c r="AF58" s="131"/>
-      <c r="AG58" s="130"/>
-      <c r="AH58" s="130"/>
-      <c r="AI58" s="130"/>
-      <c r="AJ58" s="136"/>
+      <c r="AA58" s="120"/>
+      <c r="AB58" s="120"/>
+      <c r="AC58" s="120"/>
+      <c r="AD58" s="120"/>
+      <c r="AE58" s="125"/>
+      <c r="AF58" s="121"/>
+      <c r="AG58" s="120"/>
+      <c r="AH58" s="120"/>
+      <c r="AI58" s="120"/>
+      <c r="AJ58" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="P19:R19"/>
     <mergeCell ref="V19:X19"/>
     <mergeCell ref="AB19:AD19"/>
     <mergeCell ref="AH19:AJ19"/>
@@ -5562,11 +5525,6 @@
     <mergeCell ref="V13:X13"/>
     <mergeCell ref="AB13:AD13"/>
     <mergeCell ref="AH13:AJ13"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="P19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[zssapp] change print setup to make sheet 1 of demo_sample.xlsx be printed in one page
</commit_message>
<xml_diff>
--- a/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
+++ b/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
@@ -1102,6 +1102,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1115,9 +1118,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,7 +1192,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.7330779054916986"/>
-          <c:y val="0.30801248699271666"/>
+          <c:y val="0.30801248699271694"/>
           <c:w val="0.23499361430395913"/>
           <c:h val="0.37044745057232054"/>
         </c:manualLayout>
@@ -1213,7 +1213,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1543,19 +1543,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J4"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="5" width="3.42578125" customWidth="1"/>
     <col min="6" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75">
@@ -2430,8 +2429,9 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B12:E12"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="93" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2547,48 +2547,48 @@
       <c r="D3" s="101"/>
       <c r="E3" s="101"/>
       <c r="F3" s="101"/>
-      <c r="G3" s="134" t="s">
+      <c r="G3" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="134" t="s">
+      <c r="H3" s="136"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="136"/>
+      <c r="K3" s="136"/>
+      <c r="L3" s="136"/>
+      <c r="M3" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135" t="s">
+      <c r="N3" s="136"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="134" t="s">
+      <c r="Q3" s="136"/>
+      <c r="R3" s="136"/>
+      <c r="S3" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="135"/>
-      <c r="U3" s="135"/>
-      <c r="V3" s="135"/>
-      <c r="W3" s="135"/>
-      <c r="X3" s="135"/>
-      <c r="Y3" s="134" t="s">
+      <c r="T3" s="136"/>
+      <c r="U3" s="136"/>
+      <c r="V3" s="136"/>
+      <c r="W3" s="136"/>
+      <c r="X3" s="136"/>
+      <c r="Y3" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="135"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="135"/>
-      <c r="AC3" s="135"/>
-      <c r="AD3" s="135"/>
-      <c r="AE3" s="134" t="s">
+      <c r="Z3" s="136"/>
+      <c r="AA3" s="136"/>
+      <c r="AB3" s="136"/>
+      <c r="AC3" s="136"/>
+      <c r="AD3" s="136"/>
+      <c r="AE3" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="135"/>
-      <c r="AG3" s="135"/>
-      <c r="AH3" s="135"/>
-      <c r="AI3" s="135"/>
-      <c r="AJ3" s="136"/>
+      <c r="AF3" s="136"/>
+      <c r="AG3" s="136"/>
+      <c r="AH3" s="136"/>
+      <c r="AI3" s="136"/>
+      <c r="AJ3" s="137"/>
     </row>
     <row r="4" spans="2:36">
       <c r="B4" s="102" t="s">
@@ -3110,48 +3110,48 @@
       <c r="G13" s="18"/>
       <c r="H13" s="19"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="131">
+      <c r="J13" s="132">
         <f>Input!F20</f>
         <v>23000</v>
       </c>
-      <c r="K13" s="132"/>
-      <c r="L13" s="132"/>
+      <c r="K13" s="133"/>
+      <c r="L13" s="133"/>
       <c r="M13" s="48"/>
       <c r="N13" s="19"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="131">
+      <c r="P13" s="132">
         <f>Input!G20</f>
         <v>25000</v>
       </c>
-      <c r="Q13" s="132"/>
-      <c r="R13" s="132"/>
+      <c r="Q13" s="133"/>
+      <c r="R13" s="133"/>
       <c r="S13" s="48"/>
       <c r="T13" s="19"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="131">
+      <c r="V13" s="132">
         <f>Input!H20</f>
         <v>22500</v>
       </c>
-      <c r="W13" s="132"/>
-      <c r="X13" s="132"/>
+      <c r="W13" s="133"/>
+      <c r="X13" s="133"/>
       <c r="Y13" s="48"/>
       <c r="Z13" s="19"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="131">
+      <c r="AB13" s="132">
         <f>Input!I20</f>
         <v>25600</v>
       </c>
-      <c r="AC13" s="132"/>
-      <c r="AD13" s="132"/>
+      <c r="AC13" s="133"/>
+      <c r="AD13" s="133"/>
       <c r="AE13" s="48"/>
       <c r="AF13" s="19"/>
       <c r="AG13" s="2"/>
-      <c r="AH13" s="131">
+      <c r="AH13" s="132">
         <f>Input!J20</f>
         <v>25600</v>
       </c>
-      <c r="AI13" s="132"/>
-      <c r="AJ13" s="133"/>
+      <c r="AI13" s="133"/>
+      <c r="AJ13" s="134"/>
     </row>
     <row r="14" spans="2:36">
       <c r="B14" s="106"/>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="18" spans="2:36">
       <c r="B18" s="106"/>
-      <c r="C18" s="137" t="s">
+      <c r="C18" s="131" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -3451,7 +3451,7 @@
     </row>
     <row r="19" spans="2:36">
       <c r="B19" s="106"/>
-      <c r="C19" s="137"/>
+      <c r="C19" s="131"/>
       <c r="D19" s="2"/>
       <c r="E19" s="27" t="s">
         <v>20</v>
@@ -3460,48 +3460,48 @@
       <c r="G19" s="18"/>
       <c r="H19" s="19"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="131">
+      <c r="J19" s="132">
         <f>Input!F15</f>
         <v>125000</v>
       </c>
-      <c r="K19" s="132"/>
-      <c r="L19" s="132"/>
+      <c r="K19" s="133"/>
+      <c r="L19" s="133"/>
       <c r="M19" s="48"/>
       <c r="N19" s="19"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="131">
+      <c r="P19" s="132">
         <f>Input!G15</f>
         <v>126000</v>
       </c>
-      <c r="Q19" s="132"/>
-      <c r="R19" s="132"/>
+      <c r="Q19" s="133"/>
+      <c r="R19" s="133"/>
       <c r="S19" s="48"/>
       <c r="T19" s="19"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="131">
+      <c r="V19" s="132">
         <f>Input!H15</f>
         <v>126500</v>
       </c>
-      <c r="W19" s="132"/>
-      <c r="X19" s="132"/>
+      <c r="W19" s="133"/>
+      <c r="X19" s="133"/>
       <c r="Y19" s="48"/>
       <c r="Z19" s="19"/>
       <c r="AA19" s="2"/>
-      <c r="AB19" s="131">
+      <c r="AB19" s="132">
         <f>Input!I15</f>
         <v>136000</v>
       </c>
-      <c r="AC19" s="132"/>
-      <c r="AD19" s="132"/>
+      <c r="AC19" s="133"/>
+      <c r="AD19" s="133"/>
       <c r="AE19" s="48"/>
       <c r="AF19" s="25"/>
       <c r="AG19" s="2"/>
-      <c r="AH19" s="131">
+      <c r="AH19" s="132">
         <f>Input!J15</f>
         <v>136000</v>
       </c>
-      <c r="AI19" s="132"/>
-      <c r="AJ19" s="133"/>
+      <c r="AI19" s="133"/>
+      <c r="AJ19" s="134"/>
     </row>
     <row r="20" spans="2:36">
       <c r="B20" s="106"/>
@@ -3730,7 +3730,7 @@
     </row>
     <row r="25" spans="2:36">
       <c r="B25" s="106"/>
-      <c r="C25" s="137" t="s">
+      <c r="C25" s="131" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -3813,7 +3813,7 @@
     </row>
     <row r="26" spans="2:36">
       <c r="B26" s="106"/>
-      <c r="C26" s="137"/>
+      <c r="C26" s="131"/>
       <c r="D26" s="2"/>
       <c r="E26" s="27" t="s">
         <v>22</v>
@@ -4818,7 +4818,7 @@
     </row>
     <row r="46" spans="2:36">
       <c r="B46" s="106"/>
-      <c r="C46" s="137" t="s">
+      <c r="C46" s="131" t="s">
         <v>29</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -4901,7 +4901,7 @@
     </row>
     <row r="47" spans="2:36">
       <c r="B47" s="106"/>
-      <c r="C47" s="137"/>
+      <c r="C47" s="131"/>
       <c r="D47" s="2"/>
       <c r="E47" s="27" t="s">
         <v>31</v>
@@ -5507,11 +5507,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="P19:R19"/>
     <mergeCell ref="V19:X19"/>
     <mergeCell ref="AB19:AD19"/>
     <mergeCell ref="AH19:AJ19"/>
@@ -5525,6 +5520,11 @@
     <mergeCell ref="V13:X13"/>
     <mergeCell ref="AB13:AD13"/>
     <mergeCell ref="AH13:AJ13"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="P19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix formula at "Annual" column in demo_sample Excel file
</commit_message>
<xml_diff>
--- a/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
+++ b/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
@@ -211,10 +211,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -788,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -957,9 +956,6 @@
     <xf numFmtId="3" fontId="11" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -972,22 +968,13 @@
     <xf numFmtId="3" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="11" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1022,9 +1009,6 @@
     <xf numFmtId="3" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1102,9 +1086,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1118,6 +1099,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1165,13 +1149,13 @@
                 <c:formatCode>"$"#,##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>136000</c:v>
+                  <c:v>513500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110000</c:v>
+                  <c:v>485000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26000</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1192,7 +1176,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.7330779054916986"/>
-          <c:y val="0.30801248699271694"/>
+          <c:y val="0.30801248699271705"/>
           <c:w val="0.23499361430395913"/>
           <c:h val="0.37044745057232054"/>
         </c:manualLayout>
@@ -1213,7 +1197,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1543,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1593,17 +1577,17 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="2:10" ht="29.25" customHeight="1">
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="123" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="129"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="52"/>
@@ -1617,12 +1601,12 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="30">
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="130"/>
-      <c r="D6" s="130"/>
-      <c r="E6" s="130"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
       <c r="F6" s="53" t="s">
         <v>36</v>
       </c>
@@ -1683,7 +1667,7 @@
       <c r="C10" s="65"/>
       <c r="D10" s="65"/>
       <c r="E10" s="66"/>
-      <c r="F10" s="67">
+      <c r="F10" s="63">
         <v>25000</v>
       </c>
       <c r="G10" s="54"/>
@@ -1703,12 +1687,12 @@
       <c r="J11" s="52"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="130"/>
-      <c r="D12" s="130"/>
-      <c r="E12" s="130"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="125"/>
       <c r="F12" s="69" t="s">
         <v>2</v>
       </c>
@@ -1744,9 +1728,9 @@
       <c r="I13" s="71">
         <v>56000</v>
       </c>
-      <c r="J13" s="72">
-        <f>+I13</f>
-        <v>56000</v>
+      <c r="J13" s="74">
+        <f>SUM(F13:I13)</f>
+        <v>193500</v>
       </c>
     </row>
     <row r="14" spans="2:10">
@@ -1756,21 +1740,21 @@
       <c r="C14" s="61"/>
       <c r="D14" s="61"/>
       <c r="E14" s="62"/>
-      <c r="F14" s="73">
+      <c r="F14" s="72">
         <v>80000</v>
       </c>
-      <c r="G14" s="73">
+      <c r="G14" s="72">
         <v>80000</v>
       </c>
-      <c r="H14" s="73">
+      <c r="H14" s="72">
         <v>80000</v>
       </c>
-      <c r="I14" s="74">
+      <c r="I14" s="73">
         <v>80000</v>
       </c>
-      <c r="J14" s="75">
-        <f>+I14</f>
-        <v>80000</v>
+      <c r="J14" s="74">
+        <f t="shared" ref="J14:J29" si="0">SUM(F14:I14)</f>
+        <v>320000</v>
       </c>
     </row>
     <row r="15" spans="2:10">
@@ -1780,25 +1764,25 @@
       <c r="C15" s="61"/>
       <c r="D15" s="61"/>
       <c r="E15" s="62"/>
-      <c r="F15" s="76">
+      <c r="F15" s="75">
         <f>F13+F14</f>
         <v>125000</v>
       </c>
-      <c r="G15" s="76">
+      <c r="G15" s="75">
         <f>G13+G14</f>
         <v>126000</v>
       </c>
-      <c r="H15" s="76">
+      <c r="H15" s="75">
         <f>H13+H14</f>
         <v>126500</v>
       </c>
-      <c r="I15" s="76">
+      <c r="I15" s="75">
         <f>I13+I14</f>
         <v>136000</v>
       </c>
-      <c r="J15" s="77">
-        <f>I15</f>
-        <v>136000</v>
+      <c r="J15" s="74">
+        <f t="shared" si="0"/>
+        <v>513500</v>
       </c>
     </row>
     <row r="16" spans="2:10">
@@ -1808,25 +1792,25 @@
       <c r="C16" s="61"/>
       <c r="D16" s="61"/>
       <c r="E16" s="62"/>
-      <c r="F16" s="76">
+      <c r="F16" s="75">
         <f>AVERAGE($F$8,F15)</f>
         <v>122500</v>
       </c>
-      <c r="G16" s="76">
+      <c r="G16" s="75">
         <f>AVERAGE($F$8,G15)</f>
         <v>123000</v>
       </c>
-      <c r="H16" s="76">
+      <c r="H16" s="75">
         <f>AVERAGE($F$8,H15)</f>
         <v>123250</v>
       </c>
-      <c r="I16" s="76">
+      <c r="I16" s="75">
         <f>AVERAGE($F$8,I15)</f>
         <v>128000</v>
       </c>
-      <c r="J16" s="77">
-        <f t="shared" ref="J16:J25" si="0">I16</f>
-        <v>128000</v>
+      <c r="J16" s="74">
+        <f t="shared" si="0"/>
+        <v>496750</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -1836,21 +1820,21 @@
       <c r="C17" s="61"/>
       <c r="D17" s="61"/>
       <c r="E17" s="62"/>
-      <c r="F17" s="73">
+      <c r="F17" s="72">
         <v>15000</v>
       </c>
-      <c r="G17" s="73">
+      <c r="G17" s="72">
         <v>18000</v>
       </c>
-      <c r="H17" s="73">
+      <c r="H17" s="72">
         <v>16500</v>
       </c>
-      <c r="I17" s="74">
+      <c r="I17" s="73">
         <v>14350</v>
       </c>
-      <c r="J17" s="77">
+      <c r="J17" s="74">
         <f t="shared" si="0"/>
-        <v>14350</v>
+        <v>63850</v>
       </c>
     </row>
     <row r="18" spans="2:10">
@@ -1860,21 +1844,21 @@
       <c r="C18" s="61"/>
       <c r="D18" s="61"/>
       <c r="E18" s="62"/>
-      <c r="F18" s="73">
+      <c r="F18" s="72">
         <v>15000</v>
       </c>
-      <c r="G18" s="73">
+      <c r="G18" s="72">
         <v>18000</v>
       </c>
-      <c r="H18" s="73">
+      <c r="H18" s="72">
         <v>16500</v>
       </c>
-      <c r="I18" s="74">
+      <c r="I18" s="73">
         <v>14350</v>
       </c>
-      <c r="J18" s="77">
+      <c r="J18" s="74">
         <f t="shared" si="0"/>
-        <v>14350</v>
+        <v>63850</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -1884,25 +1868,25 @@
       <c r="C19" s="61"/>
       <c r="D19" s="61"/>
       <c r="E19" s="62"/>
-      <c r="F19" s="76">
+      <c r="F19" s="75">
         <f>AVERAGE($F$7,F18)</f>
         <v>13750</v>
       </c>
-      <c r="G19" s="76">
+      <c r="G19" s="75">
         <f>AVERAGE($F$7,G18)</f>
         <v>15250</v>
       </c>
-      <c r="H19" s="76">
+      <c r="H19" s="75">
         <f>AVERAGE($F$7,H18)</f>
         <v>14500</v>
       </c>
-      <c r="I19" s="76">
+      <c r="I19" s="75">
         <f>AVERAGE($F$7,I18)</f>
         <v>13425</v>
       </c>
-      <c r="J19" s="77">
+      <c r="J19" s="74">
         <f t="shared" si="0"/>
-        <v>13425</v>
+        <v>56925</v>
       </c>
     </row>
     <row r="20" spans="2:10">
@@ -1912,21 +1896,21 @@
       <c r="C20" s="61"/>
       <c r="D20" s="61"/>
       <c r="E20" s="62"/>
-      <c r="F20" s="73">
+      <c r="F20" s="72">
         <v>23000</v>
       </c>
-      <c r="G20" s="73">
+      <c r="G20" s="72">
         <v>25000</v>
       </c>
-      <c r="H20" s="73">
+      <c r="H20" s="72">
         <v>22500</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="73">
         <v>25600</v>
       </c>
-      <c r="J20" s="77">
+      <c r="J20" s="74">
         <f t="shared" si="0"/>
-        <v>25600</v>
+        <v>96100</v>
       </c>
     </row>
     <row r="21" spans="2:10">
@@ -1936,21 +1920,21 @@
       <c r="C21" s="61"/>
       <c r="D21" s="61"/>
       <c r="E21" s="62"/>
-      <c r="F21" s="73">
+      <c r="F21" s="72">
         <v>125000</v>
       </c>
-      <c r="G21" s="73">
+      <c r="G21" s="72">
         <v>125000</v>
       </c>
-      <c r="H21" s="73">
+      <c r="H21" s="72">
         <v>125000</v>
       </c>
-      <c r="I21" s="74">
+      <c r="I21" s="73">
         <v>110000</v>
       </c>
-      <c r="J21" s="77">
+      <c r="J21" s="74">
         <f t="shared" si="0"/>
-        <v>110000</v>
+        <v>485000</v>
       </c>
     </row>
     <row r="22" spans="2:10">
@@ -1960,21 +1944,21 @@
       <c r="C22" s="61"/>
       <c r="D22" s="61"/>
       <c r="E22" s="62"/>
-      <c r="F22" s="73">
+      <c r="F22" s="72">
         <v>28000</v>
       </c>
-      <c r="G22" s="73">
+      <c r="G22" s="72">
         <v>30900</v>
       </c>
-      <c r="H22" s="73">
+      <c r="H22" s="72">
         <v>32000</v>
       </c>
-      <c r="I22" s="74">
+      <c r="I22" s="73">
         <v>26000</v>
       </c>
-      <c r="J22" s="77">
+      <c r="J22" s="74">
         <f t="shared" si="0"/>
-        <v>26000</v>
+        <v>116900</v>
       </c>
     </row>
     <row r="23" spans="2:10">
@@ -1984,21 +1968,21 @@
       <c r="C23" s="61"/>
       <c r="D23" s="61"/>
       <c r="E23" s="62"/>
-      <c r="F23" s="73">
+      <c r="F23" s="72">
         <v>25000</v>
       </c>
-      <c r="G23" s="73">
+      <c r="G23" s="72">
         <v>25000</v>
       </c>
-      <c r="H23" s="73">
+      <c r="H23" s="72">
         <v>25000</v>
       </c>
-      <c r="I23" s="74">
+      <c r="I23" s="73">
         <v>25000</v>
       </c>
-      <c r="J23" s="76">
+      <c r="J23" s="74">
         <f t="shared" si="0"/>
-        <v>25000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -2008,25 +1992,25 @@
       <c r="C24" s="61"/>
       <c r="D24" s="61"/>
       <c r="E24" s="62"/>
-      <c r="F24" s="76">
+      <c r="F24" s="75">
         <f>AVERAGE($F$10,F23)</f>
         <v>25000</v>
       </c>
-      <c r="G24" s="76">
+      <c r="G24" s="75">
         <f>AVERAGE($F$10,G23)</f>
         <v>25000</v>
       </c>
-      <c r="H24" s="76">
+      <c r="H24" s="75">
         <f>AVERAGE($F$10,H23)</f>
         <v>25000</v>
       </c>
-      <c r="I24" s="76">
+      <c r="I24" s="75">
         <f>AVERAGE($F$10,I23)</f>
         <v>25000</v>
       </c>
-      <c r="J24" s="76">
+      <c r="J24" s="74">
         <f t="shared" si="0"/>
-        <v>25000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="25" spans="2:10">
@@ -2036,25 +2020,25 @@
       <c r="C25" s="61"/>
       <c r="D25" s="61"/>
       <c r="E25" s="62"/>
-      <c r="F25" s="76">
+      <c r="F25" s="75">
         <f>AVERAGE($F$9,F22)</f>
         <v>28500</v>
       </c>
-      <c r="G25" s="76">
+      <c r="G25" s="75">
         <f>AVERAGE($F$9,G22)</f>
         <v>29950</v>
       </c>
-      <c r="H25" s="76">
+      <c r="H25" s="75">
         <f>AVERAGE($F$9,H22)</f>
         <v>30500</v>
       </c>
-      <c r="I25" s="76">
+      <c r="I25" s="75">
         <f>AVERAGE($F$9,I22)</f>
         <v>27500</v>
       </c>
-      <c r="J25" s="77">
+      <c r="J25" s="74">
         <f t="shared" si="0"/>
-        <v>27500</v>
+        <v>116450</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -2064,21 +2048,21 @@
       <c r="C26" s="61"/>
       <c r="D26" s="61"/>
       <c r="E26" s="62"/>
-      <c r="F26" s="78">
+      <c r="F26" s="76">
         <v>10</v>
       </c>
-      <c r="G26" s="78">
+      <c r="G26" s="76">
         <v>10</v>
       </c>
-      <c r="H26" s="78">
+      <c r="H26" s="76">
         <v>10</v>
       </c>
-      <c r="I26" s="79">
+      <c r="I26" s="77">
         <v>10</v>
       </c>
-      <c r="J26" s="80">
-        <f>+I26</f>
-        <v>10</v>
+      <c r="J26" s="74">
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="2:10">
@@ -2088,20 +2072,20 @@
       <c r="C27" s="61"/>
       <c r="D27" s="61"/>
       <c r="E27" s="62"/>
-      <c r="F27" s="73">
+      <c r="F27" s="72">
         <v>175000</v>
       </c>
-      <c r="G27" s="73">
+      <c r="G27" s="72">
         <v>186000</v>
       </c>
-      <c r="H27" s="73">
+      <c r="H27" s="72">
         <v>169000</v>
       </c>
-      <c r="I27" s="74">
+      <c r="I27" s="73">
         <v>155000</v>
       </c>
-      <c r="J27" s="75">
-        <f>SUM(F27:I27)</f>
+      <c r="J27" s="74">
+        <f t="shared" si="0"/>
         <v>685000</v>
       </c>
     </row>
@@ -2112,25 +2096,25 @@
       <c r="C28" s="61"/>
       <c r="D28" s="61"/>
       <c r="E28" s="62"/>
-      <c r="F28" s="81">
+      <c r="F28" s="78">
         <f>F27/F24</f>
         <v>7</v>
       </c>
-      <c r="G28" s="81">
+      <c r="G28" s="78">
         <f>G27/G24</f>
         <v>7.44</v>
       </c>
-      <c r="H28" s="81">
+      <c r="H28" s="78">
         <f>H27/H24</f>
         <v>6.76</v>
       </c>
-      <c r="I28" s="81">
+      <c r="I28" s="78">
         <f>I27/I24</f>
         <v>6.2</v>
       </c>
-      <c r="J28" s="82">
-        <f>J27/J24</f>
-        <v>27.4</v>
+      <c r="J28" s="74">
+        <f t="shared" si="0"/>
+        <v>27.400000000000002</v>
       </c>
     </row>
     <row r="29" spans="2:10">
@@ -2140,55 +2124,55 @@
       <c r="C29" s="61"/>
       <c r="D29" s="61"/>
       <c r="E29" s="62"/>
-      <c r="F29" s="73">
+      <c r="F29" s="72">
         <v>5000</v>
       </c>
-      <c r="G29" s="73">
+      <c r="G29" s="72">
         <v>5000</v>
       </c>
-      <c r="H29" s="73">
+      <c r="H29" s="72">
         <v>5000</v>
       </c>
-      <c r="I29" s="74">
+      <c r="I29" s="73">
         <v>5000</v>
       </c>
-      <c r="J29" s="75">
-        <f>SUM(F29:I29)</f>
+      <c r="J29" s="74">
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="83"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="85"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="86"/>
-      <c r="H30" s="86"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="88"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="84"/>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="89" t="s">
+      <c r="B31" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="92">
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="88">
         <v>145000</v>
       </c>
-      <c r="G31" s="92">
+      <c r="G31" s="88">
         <v>156000</v>
       </c>
-      <c r="H31" s="92">
+      <c r="H31" s="88">
         <v>135600</v>
       </c>
-      <c r="I31" s="93">
+      <c r="I31" s="89">
         <v>125000</v>
       </c>
-      <c r="J31" s="75">
-        <f t="shared" ref="J31:J38" si="1">SUM(F31:I31)</f>
+      <c r="J31" s="74">
+        <f t="shared" ref="J31:J41" si="1">SUM(F31:I31)</f>
         <v>561600</v>
       </c>
     </row>
@@ -2199,19 +2183,19 @@
       <c r="C32" s="61"/>
       <c r="D32" s="61"/>
       <c r="E32" s="62"/>
-      <c r="F32" s="73">
+      <c r="F32" s="72">
         <v>68000</v>
       </c>
-      <c r="G32" s="73">
+      <c r="G32" s="72">
         <v>68000</v>
       </c>
-      <c r="H32" s="73">
+      <c r="H32" s="72">
         <v>68000</v>
       </c>
-      <c r="I32" s="74">
+      <c r="I32" s="73">
         <v>68000</v>
       </c>
-      <c r="J32" s="75">
+      <c r="J32" s="74">
         <f t="shared" si="1"/>
         <v>272000</v>
       </c>
@@ -2223,23 +2207,23 @@
       <c r="C33" s="61"/>
       <c r="D33" s="61"/>
       <c r="E33" s="62"/>
-      <c r="F33" s="76">
+      <c r="F33" s="75">
         <f>F31-F32</f>
         <v>77000</v>
       </c>
-      <c r="G33" s="76">
+      <c r="G33" s="75">
         <f>G31-G32</f>
         <v>88000</v>
       </c>
-      <c r="H33" s="76">
+      <c r="H33" s="75">
         <f>H31-H32</f>
         <v>67600</v>
       </c>
-      <c r="I33" s="76">
+      <c r="I33" s="75">
         <f>I31-I32</f>
         <v>57000</v>
       </c>
-      <c r="J33" s="75">
+      <c r="J33" s="74">
         <f t="shared" si="1"/>
         <v>289600</v>
       </c>
@@ -2251,19 +2235,19 @@
       <c r="C34" s="61"/>
       <c r="D34" s="61"/>
       <c r="E34" s="62"/>
-      <c r="F34" s="73">
+      <c r="F34" s="72">
         <v>18000</v>
       </c>
-      <c r="G34" s="73">
+      <c r="G34" s="72">
         <v>18000</v>
       </c>
-      <c r="H34" s="73">
+      <c r="H34" s="72">
         <v>18000</v>
       </c>
-      <c r="I34" s="74">
+      <c r="I34" s="73">
         <v>18000</v>
       </c>
-      <c r="J34" s="75">
+      <c r="J34" s="74">
         <f t="shared" si="1"/>
         <v>72000</v>
       </c>
@@ -2275,19 +2259,19 @@
       <c r="C35" s="61"/>
       <c r="D35" s="61"/>
       <c r="E35" s="62"/>
-      <c r="F35" s="73">
+      <c r="F35" s="72">
         <v>11000</v>
       </c>
-      <c r="G35" s="73">
+      <c r="G35" s="72">
         <v>11000</v>
       </c>
-      <c r="H35" s="73">
+      <c r="H35" s="72">
         <v>11000</v>
       </c>
-      <c r="I35" s="74">
+      <c r="I35" s="73">
         <v>11000</v>
       </c>
-      <c r="J35" s="75">
+      <c r="J35" s="74">
         <f t="shared" si="1"/>
         <v>44000</v>
       </c>
@@ -2299,19 +2283,19 @@
       <c r="C36" s="61"/>
       <c r="D36" s="61"/>
       <c r="E36" s="62"/>
-      <c r="F36" s="73">
+      <c r="F36" s="72">
         <v>132000</v>
       </c>
-      <c r="G36" s="73">
+      <c r="G36" s="72">
         <v>127000</v>
       </c>
-      <c r="H36" s="73">
+      <c r="H36" s="72">
         <v>114500</v>
       </c>
-      <c r="I36" s="74">
+      <c r="I36" s="73">
         <v>98000</v>
       </c>
-      <c r="J36" s="75">
+      <c r="J36" s="74">
         <f t="shared" si="1"/>
         <v>471500</v>
       </c>
@@ -2323,19 +2307,19 @@
       <c r="C37" s="61"/>
       <c r="D37" s="61"/>
       <c r="E37" s="62"/>
-      <c r="F37" s="73">
+      <c r="F37" s="72">
         <v>24000</v>
       </c>
-      <c r="G37" s="73">
+      <c r="G37" s="72">
         <v>24000</v>
       </c>
-      <c r="H37" s="73">
+      <c r="H37" s="72">
         <v>24000</v>
       </c>
-      <c r="I37" s="74">
+      <c r="I37" s="73">
         <v>24000</v>
       </c>
-      <c r="J37" s="75">
+      <c r="J37" s="74">
         <f t="shared" si="1"/>
         <v>96000</v>
       </c>
@@ -2347,33 +2331,33 @@
       <c r="C38" s="61"/>
       <c r="D38" s="61"/>
       <c r="E38" s="62"/>
-      <c r="F38" s="73">
+      <c r="F38" s="72">
         <v>89000</v>
       </c>
-      <c r="G38" s="73">
+      <c r="G38" s="72">
         <v>87000</v>
       </c>
-      <c r="H38" s="73">
+      <c r="H38" s="72">
         <v>95000</v>
       </c>
-      <c r="I38" s="74">
+      <c r="I38" s="73">
         <v>65000</v>
       </c>
-      <c r="J38" s="75">
+      <c r="J38" s="74">
         <f t="shared" si="1"/>
         <v>336000</v>
       </c>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="94"/>
+      <c r="B39" s="90"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="96"/>
-      <c r="G39" s="96"/>
-      <c r="H39" s="96"/>
-      <c r="I39" s="96"/>
-      <c r="J39" s="97"/>
+      <c r="E39" s="91"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="92"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="93"/>
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="60" t="s">
@@ -2382,21 +2366,21 @@
       <c r="C40" s="61"/>
       <c r="D40" s="61"/>
       <c r="E40" s="62"/>
-      <c r="F40" s="73">
+      <c r="F40" s="72">
         <v>25000</v>
       </c>
-      <c r="G40" s="73">
+      <c r="G40" s="72">
         <v>24000</v>
       </c>
-      <c r="H40" s="73">
+      <c r="H40" s="72">
         <v>23000</v>
       </c>
-      <c r="I40" s="74">
+      <c r="I40" s="73">
         <v>22000</v>
       </c>
-      <c r="J40" s="75">
-        <f>+I40</f>
-        <v>22000</v>
+      <c r="J40" s="74">
+        <f>SUM(F40:I40)</f>
+        <v>94000</v>
       </c>
     </row>
     <row r="41" spans="2:10">
@@ -2415,12 +2399,12 @@
       <c r="H41" s="67">
         <v>65000</v>
       </c>
-      <c r="I41" s="98">
+      <c r="I41" s="94">
         <v>65000</v>
       </c>
-      <c r="J41" s="99">
-        <f>+I41</f>
-        <v>65000</v>
+      <c r="J41" s="74">
+        <f t="shared" si="1"/>
+        <v>260000</v>
       </c>
     </row>
   </sheetData>
@@ -2439,8 +2423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AJ58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView showGridLines="0" topLeftCell="E29" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2540,58 +2524,58 @@
       <c r="AJ2" s="3"/>
     </row>
     <row r="3" spans="2:36">
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="135" t="s">
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="136"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="135" t="s">
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="136"/>
-      <c r="O3" s="136"/>
-      <c r="P3" s="136" t="s">
+      <c r="N3" s="130"/>
+      <c r="O3" s="130"/>
+      <c r="P3" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="136"/>
-      <c r="R3" s="136"/>
-      <c r="S3" s="135" t="s">
+      <c r="Q3" s="130"/>
+      <c r="R3" s="130"/>
+      <c r="S3" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="136"/>
-      <c r="U3" s="136"/>
-      <c r="V3" s="136"/>
-      <c r="W3" s="136"/>
-      <c r="X3" s="136"/>
-      <c r="Y3" s="135" t="s">
+      <c r="T3" s="130"/>
+      <c r="U3" s="130"/>
+      <c r="V3" s="130"/>
+      <c r="W3" s="130"/>
+      <c r="X3" s="130"/>
+      <c r="Y3" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="136"/>
-      <c r="AA3" s="136"/>
-      <c r="AB3" s="136"/>
-      <c r="AC3" s="136"/>
-      <c r="AD3" s="136"/>
-      <c r="AE3" s="135" t="s">
+      <c r="Z3" s="130"/>
+      <c r="AA3" s="130"/>
+      <c r="AB3" s="130"/>
+      <c r="AC3" s="130"/>
+      <c r="AD3" s="130"/>
+      <c r="AE3" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="136"/>
-      <c r="AG3" s="136"/>
-      <c r="AH3" s="136"/>
-      <c r="AI3" s="136"/>
-      <c r="AJ3" s="137"/>
+      <c r="AF3" s="130"/>
+      <c r="AG3" s="130"/>
+      <c r="AH3" s="130"/>
+      <c r="AI3" s="130"/>
+      <c r="AJ3" s="131"/>
     </row>
     <row r="4" spans="2:36">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="97" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="8"/>
@@ -2627,10 +2611,10 @@
       <c r="AG4" s="14"/>
       <c r="AH4" s="14"/>
       <c r="AI4" s="14"/>
-      <c r="AJ4" s="103"/>
+      <c r="AJ4" s="98"/>
     </row>
     <row r="5" spans="2:36">
-      <c r="B5" s="104"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="16"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2664,10 +2648,10 @@
       <c r="AG5" s="2"/>
       <c r="AH5" s="20"/>
       <c r="AI5" s="20"/>
-      <c r="AJ5" s="105"/>
+      <c r="AJ5" s="100"/>
     </row>
     <row r="6" spans="2:36">
-      <c r="B6" s="106"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="16" t="s">
         <v>8</v>
       </c>
@@ -2737,20 +2721,20 @@
       <c r="AE6" s="21"/>
       <c r="AF6" s="25">
         <f>AH6/AH7</f>
-        <v>2.1875</v>
+        <v>2.0135275754422475</v>
       </c>
       <c r="AG6" s="23" t="s">
         <v>9</v>
       </c>
       <c r="AH6" s="26">
         <f>Input!J13</f>
-        <v>56000</v>
+        <v>193500</v>
       </c>
       <c r="AI6" s="20"/>
-      <c r="AJ6" s="105"/>
+      <c r="AJ6" s="100"/>
     </row>
     <row r="7" spans="2:36">
-      <c r="B7" s="106"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="16"/>
       <c r="D7" s="2"/>
       <c r="E7" s="27" t="s">
@@ -2798,13 +2782,13 @@
       <c r="AG7" s="2"/>
       <c r="AH7" s="47">
         <f>Input!J20</f>
-        <v>25600</v>
+        <v>96100</v>
       </c>
       <c r="AI7" s="20"/>
-      <c r="AJ7" s="105"/>
+      <c r="AJ7" s="100"/>
     </row>
     <row r="8" spans="2:36">
-      <c r="B8" s="106"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
@@ -2850,17 +2834,17 @@
       <c r="AG8" s="2"/>
       <c r="AH8" s="20"/>
       <c r="AI8" s="20"/>
-      <c r="AJ8" s="105"/>
+      <c r="AJ8" s="100"/>
     </row>
     <row r="9" spans="2:36">
-      <c r="B9" s="106"/>
+      <c r="B9" s="101"/>
       <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="127"/>
+      <c r="G9" s="122"/>
       <c r="H9" s="25">
         <f>H6-H8</f>
         <v>-4.3478260869565188E-2</v>
@@ -2899,15 +2883,15 @@
       <c r="AE9" s="34"/>
       <c r="AF9" s="25">
         <f>AF6-AF8</f>
-        <v>0.1875</v>
+        <v>1.3527575442247475E-2</v>
       </c>
       <c r="AG9" s="32"/>
       <c r="AH9" s="32"/>
       <c r="AI9" s="32"/>
-      <c r="AJ9" s="107"/>
+      <c r="AJ9" s="102"/>
     </row>
     <row r="10" spans="2:36">
-      <c r="B10" s="108"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="35" t="s">
         <v>14</v>
       </c>
@@ -2952,10 +2936,10 @@
       <c r="AG10" s="38"/>
       <c r="AH10" s="38"/>
       <c r="AI10" s="38"/>
-      <c r="AJ10" s="109"/>
+      <c r="AJ10" s="104"/>
     </row>
     <row r="11" spans="2:36">
-      <c r="B11" s="106"/>
+      <c r="B11" s="101"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2989,10 +2973,10 @@
       <c r="AG11" s="32"/>
       <c r="AH11" s="32"/>
       <c r="AI11" s="32"/>
-      <c r="AJ11" s="107"/>
+      <c r="AJ11" s="102"/>
     </row>
     <row r="12" spans="2:36">
-      <c r="B12" s="106"/>
+      <c r="B12" s="101"/>
       <c r="C12" s="16" t="s">
         <v>15</v>
       </c>
@@ -3082,25 +3066,25 @@
       <c r="AE12" s="46"/>
       <c r="AF12" s="25">
         <f>(AH12-AJ12)/AH13</f>
-        <v>1.626953125</v>
+        <v>1.3491155046826222</v>
       </c>
       <c r="AG12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="AH12" s="26">
         <f>Input!J13</f>
-        <v>56000</v>
+        <v>193500</v>
       </c>
       <c r="AI12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AJ12" s="110">
+      <c r="AJ12" s="105">
         <f>Input!J18</f>
-        <v>14350</v>
+        <v>63850</v>
       </c>
     </row>
     <row r="13" spans="2:36">
-      <c r="B13" s="106"/>
+      <c r="B13" s="101"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
       <c r="E13" s="27" t="s">
@@ -3110,51 +3094,51 @@
       <c r="G13" s="18"/>
       <c r="H13" s="19"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="132">
+      <c r="J13" s="126">
         <f>Input!F20</f>
         <v>23000</v>
       </c>
-      <c r="K13" s="133"/>
-      <c r="L13" s="133"/>
+      <c r="K13" s="127"/>
+      <c r="L13" s="127"/>
       <c r="M13" s="48"/>
       <c r="N13" s="19"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="132">
+      <c r="P13" s="126">
         <f>Input!G20</f>
         <v>25000</v>
       </c>
-      <c r="Q13" s="133"/>
-      <c r="R13" s="133"/>
+      <c r="Q13" s="127"/>
+      <c r="R13" s="127"/>
       <c r="S13" s="48"/>
       <c r="T13" s="19"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="132">
+      <c r="V13" s="126">
         <f>Input!H20</f>
         <v>22500</v>
       </c>
-      <c r="W13" s="133"/>
-      <c r="X13" s="133"/>
+      <c r="W13" s="127"/>
+      <c r="X13" s="127"/>
       <c r="Y13" s="48"/>
       <c r="Z13" s="19"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="132">
+      <c r="AB13" s="126">
         <f>Input!I20</f>
         <v>25600</v>
       </c>
-      <c r="AC13" s="133"/>
-      <c r="AD13" s="133"/>
+      <c r="AC13" s="127"/>
+      <c r="AD13" s="127"/>
       <c r="AE13" s="48"/>
       <c r="AF13" s="19"/>
       <c r="AG13" s="2"/>
-      <c r="AH13" s="132">
+      <c r="AH13" s="126">
         <f>Input!J20</f>
-        <v>25600</v>
-      </c>
-      <c r="AI13" s="133"/>
-      <c r="AJ13" s="134"/>
+        <v>96100</v>
+      </c>
+      <c r="AI13" s="127"/>
+      <c r="AJ13" s="128"/>
     </row>
     <row r="14" spans="2:36">
-      <c r="B14" s="106"/>
+      <c r="B14" s="101"/>
       <c r="C14" s="16" t="s">
         <v>12</v>
       </c>
@@ -3200,10 +3184,10 @@
       <c r="AG14" s="2"/>
       <c r="AH14" s="20"/>
       <c r="AI14" s="20"/>
-      <c r="AJ14" s="105"/>
+      <c r="AJ14" s="100"/>
     </row>
     <row r="15" spans="2:36">
-      <c r="B15" s="106"/>
+      <c r="B15" s="101"/>
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
@@ -3249,15 +3233,15 @@
       <c r="AE15" s="34"/>
       <c r="AF15" s="25">
         <f>AF12-AF14</f>
-        <v>-0.373046875</v>
+        <v>-0.6508844953173778</v>
       </c>
       <c r="AG15" s="2"/>
       <c r="AH15" s="20"/>
       <c r="AI15" s="20"/>
-      <c r="AJ15" s="105"/>
+      <c r="AJ15" s="100"/>
     </row>
     <row r="16" spans="2:36">
-      <c r="B16" s="108"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="35" t="s">
         <v>14</v>
       </c>
@@ -3302,10 +3286,10 @@
       <c r="AG16" s="36"/>
       <c r="AH16" s="40"/>
       <c r="AI16" s="40"/>
-      <c r="AJ16" s="111"/>
+      <c r="AJ16" s="106"/>
     </row>
     <row r="17" spans="2:36">
-      <c r="B17" s="106"/>
+      <c r="B17" s="101"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3339,11 +3323,11 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="20"/>
       <c r="AI17" s="20"/>
-      <c r="AJ17" s="105"/>
+      <c r="AJ17" s="100"/>
     </row>
     <row r="18" spans="2:36">
-      <c r="B18" s="106"/>
-      <c r="C18" s="131" t="s">
+      <c r="B18" s="101"/>
+      <c r="C18" s="132" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -3432,26 +3416,26 @@
       <c r="AE18" s="46"/>
       <c r="AF18" s="25">
         <f>(AH18-AJ18)/AH19</f>
-        <v>0.22352941176470589</v>
+        <v>0.18967867575462513</v>
       </c>
       <c r="AG18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="AH18" s="26">
         <f>Input!J13</f>
-        <v>56000</v>
+        <v>193500</v>
       </c>
       <c r="AI18" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AJ18" s="112">
+      <c r="AJ18" s="107">
         <f>Input!J20</f>
-        <v>25600</v>
+        <v>96100</v>
       </c>
     </row>
     <row r="19" spans="2:36">
-      <c r="B19" s="106"/>
-      <c r="C19" s="131"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="132"/>
       <c r="D19" s="2"/>
       <c r="E19" s="27" t="s">
         <v>20</v>
@@ -3460,51 +3444,51 @@
       <c r="G19" s="18"/>
       <c r="H19" s="19"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="132">
+      <c r="J19" s="126">
         <f>Input!F15</f>
         <v>125000</v>
       </c>
-      <c r="K19" s="133"/>
-      <c r="L19" s="133"/>
+      <c r="K19" s="127"/>
+      <c r="L19" s="127"/>
       <c r="M19" s="48"/>
       <c r="N19" s="19"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="132">
+      <c r="P19" s="126">
         <f>Input!G15</f>
         <v>126000</v>
       </c>
-      <c r="Q19" s="133"/>
-      <c r="R19" s="133"/>
+      <c r="Q19" s="127"/>
+      <c r="R19" s="127"/>
       <c r="S19" s="48"/>
       <c r="T19" s="19"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="132">
+      <c r="V19" s="126">
         <f>Input!H15</f>
         <v>126500</v>
       </c>
-      <c r="W19" s="133"/>
-      <c r="X19" s="133"/>
+      <c r="W19" s="127"/>
+      <c r="X19" s="127"/>
       <c r="Y19" s="48"/>
       <c r="Z19" s="19"/>
       <c r="AA19" s="2"/>
-      <c r="AB19" s="132">
+      <c r="AB19" s="126">
         <f>Input!I15</f>
         <v>136000</v>
       </c>
-      <c r="AC19" s="133"/>
-      <c r="AD19" s="133"/>
+      <c r="AC19" s="127"/>
+      <c r="AD19" s="127"/>
       <c r="AE19" s="48"/>
       <c r="AF19" s="25"/>
       <c r="AG19" s="2"/>
-      <c r="AH19" s="132">
+      <c r="AH19" s="126">
         <f>Input!J15</f>
-        <v>136000</v>
-      </c>
-      <c r="AI19" s="133"/>
-      <c r="AJ19" s="134"/>
+        <v>513500</v>
+      </c>
+      <c r="AI19" s="127"/>
+      <c r="AJ19" s="128"/>
     </row>
     <row r="20" spans="2:36">
-      <c r="B20" s="106"/>
+      <c r="B20" s="101"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -3538,10 +3522,10 @@
       <c r="AG20" s="2"/>
       <c r="AH20" s="20"/>
       <c r="AI20" s="20"/>
-      <c r="AJ20" s="105"/>
+      <c r="AJ20" s="100"/>
     </row>
     <row r="21" spans="2:36">
-      <c r="B21" s="106"/>
+      <c r="B21" s="101"/>
       <c r="C21" s="16" t="s">
         <v>12</v>
       </c>
@@ -3587,10 +3571,10 @@
       <c r="AG21" s="2"/>
       <c r="AH21" s="20"/>
       <c r="AI21" s="20"/>
-      <c r="AJ21" s="105"/>
+      <c r="AJ21" s="100"/>
     </row>
     <row r="22" spans="2:36">
-      <c r="B22" s="106"/>
+      <c r="B22" s="101"/>
       <c r="C22" s="16" t="s">
         <v>13</v>
       </c>
@@ -3636,15 +3620,15 @@
       <c r="AE22" s="34"/>
       <c r="AF22" s="25">
         <f>AF18-AF21</f>
-        <v>-1.776470588235294</v>
+        <v>-1.8103213242453748</v>
       </c>
       <c r="AG22" s="2"/>
       <c r="AH22" s="20"/>
       <c r="AI22" s="20"/>
-      <c r="AJ22" s="105"/>
+      <c r="AJ22" s="100"/>
     </row>
     <row r="23" spans="2:36">
-      <c r="B23" s="108"/>
+      <c r="B23" s="103"/>
       <c r="C23" s="35" t="s">
         <v>14</v>
       </c>
@@ -3689,10 +3673,10 @@
       <c r="AG23" s="36"/>
       <c r="AH23" s="40"/>
       <c r="AI23" s="40"/>
-      <c r="AJ23" s="111"/>
+      <c r="AJ23" s="106"/>
     </row>
     <row r="24" spans="2:36">
-      <c r="B24" s="106"/>
+      <c r="B24" s="101"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -3726,11 +3710,11 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="20"/>
       <c r="AI24" s="20"/>
-      <c r="AJ24" s="105"/>
+      <c r="AJ24" s="100"/>
     </row>
     <row r="25" spans="2:36">
-      <c r="B25" s="106"/>
-      <c r="C25" s="131" t="s">
+      <c r="B25" s="101"/>
+      <c r="C25" s="132" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -3799,21 +3783,21 @@
       <c r="AE25" s="21"/>
       <c r="AF25" s="25">
         <f>AH25/AH26</f>
-        <v>1.7839721254355401</v>
+        <v>1.5050900548159749</v>
       </c>
       <c r="AG25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="AH25" s="26">
         <f>Input!J20</f>
-        <v>25600</v>
+        <v>96100</v>
       </c>
       <c r="AI25" s="20"/>
-      <c r="AJ25" s="105"/>
+      <c r="AJ25" s="100"/>
     </row>
     <row r="26" spans="2:36">
-      <c r="B26" s="106"/>
-      <c r="C26" s="131"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="132"/>
       <c r="D26" s="2"/>
       <c r="E26" s="27" t="s">
         <v>22</v>
@@ -3860,13 +3844,13 @@
       <c r="AG26" s="2"/>
       <c r="AH26" s="47">
         <f>Input!J18</f>
-        <v>14350</v>
+        <v>63850</v>
       </c>
       <c r="AI26" s="20"/>
-      <c r="AJ26" s="105"/>
+      <c r="AJ26" s="100"/>
     </row>
     <row r="27" spans="2:36">
-      <c r="B27" s="106"/>
+      <c r="B27" s="101"/>
       <c r="C27" s="49"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -3900,10 +3884,10 @@
       <c r="AG27" s="2"/>
       <c r="AH27" s="20"/>
       <c r="AI27" s="20"/>
-      <c r="AJ27" s="105"/>
+      <c r="AJ27" s="100"/>
     </row>
     <row r="28" spans="2:36">
-      <c r="B28" s="106"/>
+      <c r="B28" s="101"/>
       <c r="C28" s="16" t="s">
         <v>12</v>
       </c>
@@ -3949,10 +3933,10 @@
       <c r="AG28" s="2"/>
       <c r="AH28" s="20"/>
       <c r="AI28" s="20"/>
-      <c r="AJ28" s="105"/>
+      <c r="AJ28" s="100"/>
     </row>
     <row r="29" spans="2:36">
-      <c r="B29" s="106"/>
+      <c r="B29" s="101"/>
       <c r="C29" s="16" t="s">
         <v>13</v>
       </c>
@@ -3998,15 +3982,15 @@
       <c r="AE29" s="34"/>
       <c r="AF29" s="25">
         <f>AF25-AF28</f>
-        <v>-0.21602787456445993</v>
+        <v>-0.49490994518402509</v>
       </c>
       <c r="AG29" s="2"/>
       <c r="AH29" s="20"/>
       <c r="AI29" s="20"/>
-      <c r="AJ29" s="105"/>
+      <c r="AJ29" s="100"/>
     </row>
     <row r="30" spans="2:36">
-      <c r="B30" s="108"/>
+      <c r="B30" s="103"/>
       <c r="C30" s="35" t="s">
         <v>14</v>
       </c>
@@ -4051,10 +4035,10 @@
       <c r="AG30" s="36"/>
       <c r="AH30" s="40"/>
       <c r="AI30" s="40"/>
-      <c r="AJ30" s="111"/>
+      <c r="AJ30" s="106"/>
     </row>
     <row r="31" spans="2:36">
-      <c r="B31" s="106"/>
+      <c r="B31" s="101"/>
       <c r="C31" s="16"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -4088,10 +4072,10 @@
       <c r="AG31" s="2"/>
       <c r="AH31" s="20"/>
       <c r="AI31" s="20"/>
-      <c r="AJ31" s="105"/>
+      <c r="AJ31" s="100"/>
     </row>
     <row r="32" spans="2:36">
-      <c r="B32" s="106"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="16" t="s">
         <v>23</v>
       </c>
@@ -4161,20 +4145,20 @@
       <c r="AE32" s="21"/>
       <c r="AF32" s="25">
         <f>AH32/AH33</f>
-        <v>0.560546875</v>
+        <v>0.66441207075962538</v>
       </c>
       <c r="AG32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="AH32" s="26">
         <f>Input!J17</f>
-        <v>14350</v>
+        <v>63850</v>
       </c>
       <c r="AI32" s="20"/>
-      <c r="AJ32" s="105"/>
+      <c r="AJ32" s="100"/>
     </row>
     <row r="33" spans="2:36">
-      <c r="B33" s="106"/>
+      <c r="B33" s="101"/>
       <c r="C33" s="16"/>
       <c r="D33" s="2"/>
       <c r="E33" s="27" t="s">
@@ -4222,13 +4206,13 @@
       <c r="AG33" s="2"/>
       <c r="AH33" s="47">
         <f>Input!J20</f>
-        <v>25600</v>
+        <v>96100</v>
       </c>
       <c r="AI33" s="20"/>
-      <c r="AJ33" s="105"/>
+      <c r="AJ33" s="100"/>
     </row>
     <row r="34" spans="2:36">
-      <c r="B34" s="106"/>
+      <c r="B34" s="101"/>
       <c r="C34" s="16" t="s">
         <v>12</v>
       </c>
@@ -4274,10 +4258,10 @@
       <c r="AG34" s="2"/>
       <c r="AH34" s="20"/>
       <c r="AI34" s="20"/>
-      <c r="AJ34" s="105"/>
+      <c r="AJ34" s="100"/>
     </row>
     <row r="35" spans="2:36">
-      <c r="B35" s="106"/>
+      <c r="B35" s="101"/>
       <c r="C35" s="16" t="s">
         <v>13</v>
       </c>
@@ -4323,15 +4307,15 @@
       <c r="AE35" s="34"/>
       <c r="AF35" s="25">
         <f>AF32-AF34</f>
-        <v>-1.439453125</v>
+        <v>-1.3355879292403747</v>
       </c>
       <c r="AG35" s="2"/>
       <c r="AH35" s="20"/>
       <c r="AI35" s="20"/>
-      <c r="AJ35" s="105"/>
+      <c r="AJ35" s="100"/>
     </row>
     <row r="36" spans="2:36">
-      <c r="B36" s="108"/>
+      <c r="B36" s="103"/>
       <c r="C36" s="35" t="s">
         <v>14</v>
       </c>
@@ -4376,10 +4360,10 @@
       <c r="AG36" s="36"/>
       <c r="AH36" s="40"/>
       <c r="AI36" s="40"/>
-      <c r="AJ36" s="111"/>
+      <c r="AJ36" s="106"/>
     </row>
     <row r="37" spans="2:36">
-      <c r="B37" s="106"/>
+      <c r="B37" s="101"/>
       <c r="C37" s="16"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -4413,10 +4397,10 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="20"/>
       <c r="AI37" s="20"/>
-      <c r="AJ37" s="105"/>
+      <c r="AJ37" s="100"/>
     </row>
     <row r="38" spans="2:36">
-      <c r="B38" s="106"/>
+      <c r="B38" s="101"/>
       <c r="C38" s="16" t="s">
         <v>25</v>
       </c>
@@ -4496,10 +4480,10 @@
         <v>272000</v>
       </c>
       <c r="AI38" s="20"/>
-      <c r="AJ38" s="105"/>
+      <c r="AJ38" s="100"/>
     </row>
     <row r="39" spans="2:36">
-      <c r="B39" s="106"/>
+      <c r="B39" s="101"/>
       <c r="C39" s="16"/>
       <c r="D39" s="2"/>
       <c r="E39" s="27" t="s">
@@ -4550,10 +4534,10 @@
         <v>289600</v>
       </c>
       <c r="AI39" s="20"/>
-      <c r="AJ39" s="105"/>
+      <c r="AJ39" s="100"/>
     </row>
     <row r="40" spans="2:36">
-      <c r="B40" s="106"/>
+      <c r="B40" s="101"/>
       <c r="C40" s="16" t="s">
         <v>12</v>
       </c>
@@ -4599,10 +4583,10 @@
       <c r="AG40" s="2"/>
       <c r="AH40" s="20"/>
       <c r="AI40" s="20"/>
-      <c r="AJ40" s="105"/>
+      <c r="AJ40" s="100"/>
     </row>
     <row r="41" spans="2:36">
-      <c r="B41" s="106"/>
+      <c r="B41" s="101"/>
       <c r="C41" s="16" t="s">
         <v>13</v>
       </c>
@@ -4653,10 +4637,10 @@
       <c r="AG41" s="2"/>
       <c r="AH41" s="20"/>
       <c r="AI41" s="20"/>
-      <c r="AJ41" s="105"/>
+      <c r="AJ41" s="100"/>
     </row>
     <row r="42" spans="2:36">
-      <c r="B42" s="108"/>
+      <c r="B42" s="103"/>
       <c r="C42" s="35" t="s">
         <v>14</v>
       </c>
@@ -4701,10 +4685,10 @@
       <c r="AG42" s="36"/>
       <c r="AH42" s="40"/>
       <c r="AI42" s="40"/>
-      <c r="AJ42" s="111"/>
+      <c r="AJ42" s="106"/>
     </row>
     <row r="43" spans="2:36">
-      <c r="B43" s="106"/>
+      <c r="B43" s="101"/>
       <c r="C43" s="16"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -4738,10 +4722,10 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="20"/>
       <c r="AI43" s="20"/>
-      <c r="AJ43" s="105"/>
+      <c r="AJ43" s="100"/>
     </row>
     <row r="44" spans="2:36">
-      <c r="B44" s="113" t="s">
+      <c r="B44" s="108" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="2"/>
@@ -4777,10 +4761,10 @@
       <c r="AG44" s="2"/>
       <c r="AH44" s="20"/>
       <c r="AI44" s="20"/>
-      <c r="AJ44" s="105"/>
+      <c r="AJ44" s="100"/>
     </row>
     <row r="45" spans="2:36">
-      <c r="B45" s="106"/>
+      <c r="B45" s="101"/>
       <c r="C45" s="16"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -4814,11 +4798,11 @@
       <c r="AG45" s="2"/>
       <c r="AH45" s="20"/>
       <c r="AI45" s="20"/>
-      <c r="AJ45" s="114"/>
+      <c r="AJ45" s="109"/>
     </row>
     <row r="46" spans="2:36">
-      <c r="B46" s="106"/>
-      <c r="C46" s="131" t="s">
+      <c r="B46" s="101"/>
+      <c r="C46" s="132" t="s">
         <v>29</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -4897,11 +4881,11 @@
         <v>72000</v>
       </c>
       <c r="AI46" s="20"/>
-      <c r="AJ46" s="114"/>
+      <c r="AJ46" s="109"/>
     </row>
     <row r="47" spans="2:36">
-      <c r="B47" s="106"/>
-      <c r="C47" s="131"/>
+      <c r="B47" s="101"/>
+      <c r="C47" s="132"/>
       <c r="D47" s="2"/>
       <c r="E47" s="27" t="s">
         <v>31</v>
@@ -4951,10 +4935,10 @@
         <v>561600</v>
       </c>
       <c r="AI47" s="20"/>
-      <c r="AJ47" s="114"/>
+      <c r="AJ47" s="109"/>
     </row>
     <row r="48" spans="2:36">
-      <c r="B48" s="106"/>
+      <c r="B48" s="101"/>
       <c r="C48" s="49"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -4988,10 +4972,10 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="20"/>
       <c r="AI48" s="20"/>
-      <c r="AJ48" s="114"/>
+      <c r="AJ48" s="109"/>
     </row>
     <row r="49" spans="2:36">
-      <c r="B49" s="106"/>
+      <c r="B49" s="101"/>
       <c r="C49" s="16" t="s">
         <v>12</v>
       </c>
@@ -5037,10 +5021,10 @@
       <c r="AG49" s="2"/>
       <c r="AH49" s="20"/>
       <c r="AI49" s="20"/>
-      <c r="AJ49" s="114"/>
+      <c r="AJ49" s="109"/>
     </row>
     <row r="50" spans="2:36">
-      <c r="B50" s="106"/>
+      <c r="B50" s="101"/>
       <c r="C50" s="16" t="s">
         <v>13</v>
       </c>
@@ -5091,10 +5075,10 @@
       <c r="AG50" s="2"/>
       <c r="AH50" s="20"/>
       <c r="AI50" s="20"/>
-      <c r="AJ50" s="114"/>
+      <c r="AJ50" s="109"/>
     </row>
     <row r="51" spans="2:36">
-      <c r="B51" s="108"/>
+      <c r="B51" s="103"/>
       <c r="C51" s="35" t="s">
         <v>14</v>
       </c>
@@ -5139,10 +5123,10 @@
       <c r="AG51" s="36"/>
       <c r="AH51" s="40"/>
       <c r="AI51" s="40"/>
-      <c r="AJ51" s="115"/>
+      <c r="AJ51" s="110"/>
     </row>
     <row r="52" spans="2:36">
-      <c r="B52" s="106"/>
+      <c r="B52" s="101"/>
       <c r="C52" s="16"/>
       <c r="D52" s="32"/>
       <c r="E52" s="32"/>
@@ -5176,10 +5160,10 @@
       <c r="AG52" s="2"/>
       <c r="AH52" s="20"/>
       <c r="AI52" s="20"/>
-      <c r="AJ52" s="114"/>
+      <c r="AJ52" s="109"/>
     </row>
     <row r="53" spans="2:36">
-      <c r="B53" s="106"/>
+      <c r="B53" s="101"/>
       <c r="C53" s="16" t="s">
         <v>32</v>
       </c>
@@ -5259,10 +5243,10 @@
         <v>44000</v>
       </c>
       <c r="AI53" s="20"/>
-      <c r="AJ53" s="114"/>
+      <c r="AJ53" s="109"/>
     </row>
     <row r="54" spans="2:36">
-      <c r="B54" s="106"/>
+      <c r="B54" s="101"/>
       <c r="C54" s="16" t="s">
         <v>33</v>
       </c>
@@ -5315,10 +5299,10 @@
         <v>561600</v>
       </c>
       <c r="AI54" s="20"/>
-      <c r="AJ54" s="114"/>
+      <c r="AJ54" s="109"/>
     </row>
     <row r="55" spans="2:36">
-      <c r="B55" s="106"/>
+      <c r="B55" s="101"/>
       <c r="C55" s="16"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -5352,10 +5336,10 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="20"/>
       <c r="AI55" s="20"/>
-      <c r="AJ55" s="114"/>
+      <c r="AJ55" s="109"/>
     </row>
     <row r="56" spans="2:36">
-      <c r="B56" s="106"/>
+      <c r="B56" s="101"/>
       <c r="C56" s="16" t="s">
         <v>12</v>
       </c>
@@ -5401,10 +5385,10 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="20"/>
       <c r="AI56" s="20"/>
-      <c r="AJ56" s="114"/>
+      <c r="AJ56" s="109"/>
     </row>
     <row r="57" spans="2:36">
-      <c r="B57" s="106"/>
+      <c r="B57" s="101"/>
       <c r="C57" s="16" t="s">
         <v>13</v>
       </c>
@@ -5455,58 +5439,63 @@
       <c r="AG57" s="32"/>
       <c r="AH57" s="32"/>
       <c r="AI57" s="32"/>
-      <c r="AJ57" s="107"/>
+      <c r="AJ57" s="102"/>
     </row>
     <row r="58" spans="2:36">
-      <c r="B58" s="116"/>
-      <c r="C58" s="117" t="s">
+      <c r="B58" s="111"/>
+      <c r="C58" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="118"/>
-      <c r="E58" s="118"/>
-      <c r="F58" s="119"/>
-      <c r="G58" s="120"/>
-      <c r="H58" s="121"/>
-      <c r="I58" s="118"/>
-      <c r="J58" s="122"/>
-      <c r="K58" s="122"/>
-      <c r="L58" s="118"/>
-      <c r="M58" s="123"/>
-      <c r="N58" s="124">
+      <c r="D58" s="113"/>
+      <c r="E58" s="113"/>
+      <c r="F58" s="114"/>
+      <c r="G58" s="115"/>
+      <c r="H58" s="116"/>
+      <c r="I58" s="113"/>
+      <c r="J58" s="117"/>
+      <c r="K58" s="117"/>
+      <c r="L58" s="113"/>
+      <c r="M58" s="118"/>
+      <c r="N58" s="119">
         <f>N53-H53</f>
         <v>-5.3492484526967282E-3</v>
       </c>
-      <c r="O58" s="118"/>
-      <c r="P58" s="118"/>
-      <c r="Q58" s="118"/>
-      <c r="R58" s="120"/>
-      <c r="S58" s="125"/>
-      <c r="T58" s="124">
+      <c r="O58" s="113"/>
+      <c r="P58" s="113"/>
+      <c r="Q58" s="113"/>
+      <c r="R58" s="115"/>
+      <c r="S58" s="120"/>
+      <c r="T58" s="119">
         <f>T53-N53</f>
         <v>1.0608123439981854E-2</v>
       </c>
-      <c r="U58" s="120"/>
-      <c r="V58" s="120"/>
-      <c r="W58" s="120"/>
-      <c r="X58" s="120"/>
-      <c r="Y58" s="125"/>
-      <c r="Z58" s="124">
+      <c r="U58" s="115"/>
+      <c r="V58" s="115"/>
+      <c r="W58" s="115"/>
+      <c r="X58" s="115"/>
+      <c r="Y58" s="120"/>
+      <c r="Z58" s="119">
         <f>Z53-T53</f>
         <v>6.8790560471976292E-3</v>
       </c>
-      <c r="AA58" s="120"/>
-      <c r="AB58" s="120"/>
-      <c r="AC58" s="120"/>
-      <c r="AD58" s="120"/>
-      <c r="AE58" s="125"/>
-      <c r="AF58" s="121"/>
-      <c r="AG58" s="120"/>
-      <c r="AH58" s="120"/>
-      <c r="AI58" s="120"/>
-      <c r="AJ58" s="126"/>
+      <c r="AA58" s="115"/>
+      <c r="AB58" s="115"/>
+      <c r="AC58" s="115"/>
+      <c r="AD58" s="115"/>
+      <c r="AE58" s="120"/>
+      <c r="AF58" s="116"/>
+      <c r="AG58" s="115"/>
+      <c r="AH58" s="115"/>
+      <c r="AI58" s="115"/>
+      <c r="AJ58" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="P19:R19"/>
     <mergeCell ref="V19:X19"/>
     <mergeCell ref="AB19:AD19"/>
     <mergeCell ref="AH19:AJ19"/>
@@ -5520,11 +5509,6 @@
     <mergeCell ref="V13:X13"/>
     <mergeCell ref="AB13:AD13"/>
     <mergeCell ref="AH13:AJ13"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="P19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove some cells' style to avoid blocking overflow
</commit_message>
<xml_diff>
--- a/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
+++ b/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="22995" windowHeight="11055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -1009,12 +1009,6 @@
     <xf numFmtId="3" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1085,6 +1079,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1176,7 +1176,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.7330779054916986"/>
-          <c:y val="0.30801248699271705"/>
+          <c:y val="0.30801248699271727"/>
           <c:w val="0.23499361430395913"/>
           <c:h val="0.37044745057232054"/>
         </c:manualLayout>
@@ -1197,7 +1197,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1527,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1545,14 +1545,6 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="2:10" ht="15.75">
       <c r="B2" s="1"/>
@@ -1577,17 +1569,17 @@
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="2:10" ht="29.25" customHeight="1">
-      <c r="B4" s="123" t="s">
+      <c r="B4" s="121" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="122"/>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="52"/>
@@ -1601,12 +1593,12 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="30">
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
       <c r="F6" s="53" t="s">
         <v>36</v>
       </c>
@@ -1687,12 +1679,12 @@
       <c r="J11" s="52"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="125"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
       <c r="F12" s="69" t="s">
         <v>2</v>
       </c>
@@ -2423,15 +2415,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AJ58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E29" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
@@ -2451,23 +2443,6 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
@@ -2524,13 +2499,13 @@
       <c r="AJ2" s="3"/>
     </row>
     <row r="3" spans="2:36">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
       <c r="G3" s="129" t="s">
         <v>2</v>
       </c>
@@ -2575,7 +2550,7 @@
       <c r="AJ3" s="131"/>
     </row>
     <row r="4" spans="2:36">
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="95" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="8"/>
@@ -2611,10 +2586,10 @@
       <c r="AG4" s="14"/>
       <c r="AH4" s="14"/>
       <c r="AI4" s="14"/>
-      <c r="AJ4" s="98"/>
+      <c r="AJ4" s="96"/>
     </row>
     <row r="5" spans="2:36">
-      <c r="B5" s="99"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="16"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2648,10 +2623,10 @@
       <c r="AG5" s="2"/>
       <c r="AH5" s="20"/>
       <c r="AI5" s="20"/>
-      <c r="AJ5" s="100"/>
+      <c r="AJ5" s="98"/>
     </row>
     <row r="6" spans="2:36">
-      <c r="B6" s="101"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="16" t="s">
         <v>8</v>
       </c>
@@ -2731,10 +2706,10 @@
         <v>193500</v>
       </c>
       <c r="AI6" s="20"/>
-      <c r="AJ6" s="100"/>
+      <c r="AJ6" s="98"/>
     </row>
     <row r="7" spans="2:36">
-      <c r="B7" s="101"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="16"/>
       <c r="D7" s="2"/>
       <c r="E7" s="27" t="s">
@@ -2785,10 +2760,10 @@
         <v>96100</v>
       </c>
       <c r="AI7" s="20"/>
-      <c r="AJ7" s="100"/>
+      <c r="AJ7" s="98"/>
     </row>
     <row r="8" spans="2:36">
-      <c r="B8" s="101"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
@@ -2834,17 +2809,17 @@
       <c r="AG8" s="2"/>
       <c r="AH8" s="20"/>
       <c r="AI8" s="20"/>
-      <c r="AJ8" s="100"/>
+      <c r="AJ8" s="98"/>
     </row>
     <row r="9" spans="2:36">
-      <c r="B9" s="101"/>
+      <c r="B9" s="99"/>
       <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="122"/>
+      <c r="G9" s="120"/>
       <c r="H9" s="25">
         <f>H6-H8</f>
         <v>-4.3478260869565188E-2</v>
@@ -2888,10 +2863,10 @@
       <c r="AG9" s="32"/>
       <c r="AH9" s="32"/>
       <c r="AI9" s="32"/>
-      <c r="AJ9" s="102"/>
+      <c r="AJ9" s="100"/>
     </row>
     <row r="10" spans="2:36">
-      <c r="B10" s="103"/>
+      <c r="B10" s="101"/>
       <c r="C10" s="35" t="s">
         <v>14</v>
       </c>
@@ -2936,10 +2911,10 @@
       <c r="AG10" s="38"/>
       <c r="AH10" s="38"/>
       <c r="AI10" s="38"/>
-      <c r="AJ10" s="104"/>
+      <c r="AJ10" s="102"/>
     </row>
     <row r="11" spans="2:36">
-      <c r="B11" s="101"/>
+      <c r="B11" s="99"/>
       <c r="C11" s="16"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2973,10 +2948,10 @@
       <c r="AG11" s="32"/>
       <c r="AH11" s="32"/>
       <c r="AI11" s="32"/>
-      <c r="AJ11" s="102"/>
+      <c r="AJ11" s="100"/>
     </row>
     <row r="12" spans="2:36">
-      <c r="B12" s="101"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="16" t="s">
         <v>15</v>
       </c>
@@ -3078,13 +3053,13 @@
       <c r="AI12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AJ12" s="105">
+      <c r="AJ12" s="103">
         <f>Input!J18</f>
         <v>63850</v>
       </c>
     </row>
     <row r="13" spans="2:36">
-      <c r="B13" s="101"/>
+      <c r="B13" s="99"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
       <c r="E13" s="27" t="s">
@@ -3138,7 +3113,7 @@
       <c r="AJ13" s="128"/>
     </row>
     <row r="14" spans="2:36">
-      <c r="B14" s="101"/>
+      <c r="B14" s="99"/>
       <c r="C14" s="16" t="s">
         <v>12</v>
       </c>
@@ -3184,10 +3159,10 @@
       <c r="AG14" s="2"/>
       <c r="AH14" s="20"/>
       <c r="AI14" s="20"/>
-      <c r="AJ14" s="100"/>
+      <c r="AJ14" s="98"/>
     </row>
     <row r="15" spans="2:36">
-      <c r="B15" s="101"/>
+      <c r="B15" s="99"/>
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
@@ -3238,10 +3213,10 @@
       <c r="AG15" s="2"/>
       <c r="AH15" s="20"/>
       <c r="AI15" s="20"/>
-      <c r="AJ15" s="100"/>
+      <c r="AJ15" s="98"/>
     </row>
     <row r="16" spans="2:36">
-      <c r="B16" s="103"/>
+      <c r="B16" s="101"/>
       <c r="C16" s="35" t="s">
         <v>14</v>
       </c>
@@ -3286,10 +3261,10 @@
       <c r="AG16" s="36"/>
       <c r="AH16" s="40"/>
       <c r="AI16" s="40"/>
-      <c r="AJ16" s="106"/>
+      <c r="AJ16" s="104"/>
     </row>
     <row r="17" spans="2:36">
-      <c r="B17" s="101"/>
+      <c r="B17" s="99"/>
       <c r="C17" s="16"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3323,10 +3298,10 @@
       <c r="AG17" s="2"/>
       <c r="AH17" s="20"/>
       <c r="AI17" s="20"/>
-      <c r="AJ17" s="100"/>
+      <c r="AJ17" s="98"/>
     </row>
     <row r="18" spans="2:36">
-      <c r="B18" s="101"/>
+      <c r="B18" s="99"/>
       <c r="C18" s="132" t="s">
         <v>18</v>
       </c>
@@ -3428,13 +3403,13 @@
       <c r="AI18" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AJ18" s="107">
+      <c r="AJ18" s="105">
         <f>Input!J20</f>
         <v>96100</v>
       </c>
     </row>
     <row r="19" spans="2:36">
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="132"/>
       <c r="D19" s="2"/>
       <c r="E19" s="27" t="s">
@@ -3488,7 +3463,7 @@
       <c r="AJ19" s="128"/>
     </row>
     <row r="20" spans="2:36">
-      <c r="B20" s="101"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="16"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -3522,10 +3497,10 @@
       <c r="AG20" s="2"/>
       <c r="AH20" s="20"/>
       <c r="AI20" s="20"/>
-      <c r="AJ20" s="100"/>
+      <c r="AJ20" s="98"/>
     </row>
     <row r="21" spans="2:36">
-      <c r="B21" s="101"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="16" t="s">
         <v>12</v>
       </c>
@@ -3571,10 +3546,10 @@
       <c r="AG21" s="2"/>
       <c r="AH21" s="20"/>
       <c r="AI21" s="20"/>
-      <c r="AJ21" s="100"/>
+      <c r="AJ21" s="98"/>
     </row>
     <row r="22" spans="2:36">
-      <c r="B22" s="101"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="16" t="s">
         <v>13</v>
       </c>
@@ -3625,10 +3600,10 @@
       <c r="AG22" s="2"/>
       <c r="AH22" s="20"/>
       <c r="AI22" s="20"/>
-      <c r="AJ22" s="100"/>
+      <c r="AJ22" s="98"/>
     </row>
     <row r="23" spans="2:36">
-      <c r="B23" s="103"/>
+      <c r="B23" s="101"/>
       <c r="C23" s="35" t="s">
         <v>14</v>
       </c>
@@ -3673,10 +3648,10 @@
       <c r="AG23" s="36"/>
       <c r="AH23" s="40"/>
       <c r="AI23" s="40"/>
-      <c r="AJ23" s="106"/>
+      <c r="AJ23" s="104"/>
     </row>
     <row r="24" spans="2:36">
-      <c r="B24" s="101"/>
+      <c r="B24" s="99"/>
       <c r="C24" s="16"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -3710,10 +3685,10 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="20"/>
       <c r="AI24" s="20"/>
-      <c r="AJ24" s="100"/>
+      <c r="AJ24" s="98"/>
     </row>
     <row r="25" spans="2:36">
-      <c r="B25" s="101"/>
+      <c r="B25" s="99"/>
       <c r="C25" s="132" t="s">
         <v>21</v>
       </c>
@@ -3793,10 +3768,10 @@
         <v>96100</v>
       </c>
       <c r="AI25" s="20"/>
-      <c r="AJ25" s="100"/>
+      <c r="AJ25" s="98"/>
     </row>
     <row r="26" spans="2:36">
-      <c r="B26" s="101"/>
+      <c r="B26" s="99"/>
       <c r="C26" s="132"/>
       <c r="D26" s="2"/>
       <c r="E26" s="27" t="s">
@@ -3847,10 +3822,10 @@
         <v>63850</v>
       </c>
       <c r="AI26" s="20"/>
-      <c r="AJ26" s="100"/>
+      <c r="AJ26" s="98"/>
     </row>
     <row r="27" spans="2:36">
-      <c r="B27" s="101"/>
+      <c r="B27" s="99"/>
       <c r="C27" s="49"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -3884,10 +3859,10 @@
       <c r="AG27" s="2"/>
       <c r="AH27" s="20"/>
       <c r="AI27" s="20"/>
-      <c r="AJ27" s="100"/>
+      <c r="AJ27" s="98"/>
     </row>
     <row r="28" spans="2:36">
-      <c r="B28" s="101"/>
+      <c r="B28" s="99"/>
       <c r="C28" s="16" t="s">
         <v>12</v>
       </c>
@@ -3933,10 +3908,10 @@
       <c r="AG28" s="2"/>
       <c r="AH28" s="20"/>
       <c r="AI28" s="20"/>
-      <c r="AJ28" s="100"/>
+      <c r="AJ28" s="98"/>
     </row>
     <row r="29" spans="2:36">
-      <c r="B29" s="101"/>
+      <c r="B29" s="99"/>
       <c r="C29" s="16" t="s">
         <v>13</v>
       </c>
@@ -3987,10 +3962,10 @@
       <c r="AG29" s="2"/>
       <c r="AH29" s="20"/>
       <c r="AI29" s="20"/>
-      <c r="AJ29" s="100"/>
+      <c r="AJ29" s="98"/>
     </row>
     <row r="30" spans="2:36">
-      <c r="B30" s="103"/>
+      <c r="B30" s="101"/>
       <c r="C30" s="35" t="s">
         <v>14</v>
       </c>
@@ -4035,10 +4010,10 @@
       <c r="AG30" s="36"/>
       <c r="AH30" s="40"/>
       <c r="AI30" s="40"/>
-      <c r="AJ30" s="106"/>
+      <c r="AJ30" s="104"/>
     </row>
     <row r="31" spans="2:36">
-      <c r="B31" s="101"/>
+      <c r="B31" s="99"/>
       <c r="C31" s="16"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -4072,10 +4047,10 @@
       <c r="AG31" s="2"/>
       <c r="AH31" s="20"/>
       <c r="AI31" s="20"/>
-      <c r="AJ31" s="100"/>
+      <c r="AJ31" s="98"/>
     </row>
     <row r="32" spans="2:36">
-      <c r="B32" s="101"/>
+      <c r="B32" s="99"/>
       <c r="C32" s="16" t="s">
         <v>23</v>
       </c>
@@ -4155,10 +4130,10 @@
         <v>63850</v>
       </c>
       <c r="AI32" s="20"/>
-      <c r="AJ32" s="100"/>
+      <c r="AJ32" s="98"/>
     </row>
     <row r="33" spans="2:36">
-      <c r="B33" s="101"/>
+      <c r="B33" s="99"/>
       <c r="C33" s="16"/>
       <c r="D33" s="2"/>
       <c r="E33" s="27" t="s">
@@ -4209,10 +4184,10 @@
         <v>96100</v>
       </c>
       <c r="AI33" s="20"/>
-      <c r="AJ33" s="100"/>
+      <c r="AJ33" s="98"/>
     </row>
     <row r="34" spans="2:36">
-      <c r="B34" s="101"/>
+      <c r="B34" s="99"/>
       <c r="C34" s="16" t="s">
         <v>12</v>
       </c>
@@ -4258,10 +4233,10 @@
       <c r="AG34" s="2"/>
       <c r="AH34" s="20"/>
       <c r="AI34" s="20"/>
-      <c r="AJ34" s="100"/>
+      <c r="AJ34" s="98"/>
     </row>
     <row r="35" spans="2:36">
-      <c r="B35" s="101"/>
+      <c r="B35" s="99"/>
       <c r="C35" s="16" t="s">
         <v>13</v>
       </c>
@@ -4312,10 +4287,10 @@
       <c r="AG35" s="2"/>
       <c r="AH35" s="20"/>
       <c r="AI35" s="20"/>
-      <c r="AJ35" s="100"/>
+      <c r="AJ35" s="98"/>
     </row>
     <row r="36" spans="2:36">
-      <c r="B36" s="103"/>
+      <c r="B36" s="101"/>
       <c r="C36" s="35" t="s">
         <v>14</v>
       </c>
@@ -4360,10 +4335,10 @@
       <c r="AG36" s="36"/>
       <c r="AH36" s="40"/>
       <c r="AI36" s="40"/>
-      <c r="AJ36" s="106"/>
+      <c r="AJ36" s="104"/>
     </row>
     <row r="37" spans="2:36">
-      <c r="B37" s="101"/>
+      <c r="B37" s="99"/>
       <c r="C37" s="16"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -4397,10 +4372,10 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="20"/>
       <c r="AI37" s="20"/>
-      <c r="AJ37" s="100"/>
+      <c r="AJ37" s="98"/>
     </row>
     <row r="38" spans="2:36">
-      <c r="B38" s="101"/>
+      <c r="B38" s="99"/>
       <c r="C38" s="16" t="s">
         <v>25</v>
       </c>
@@ -4480,10 +4455,10 @@
         <v>272000</v>
       </c>
       <c r="AI38" s="20"/>
-      <c r="AJ38" s="100"/>
+      <c r="AJ38" s="98"/>
     </row>
     <row r="39" spans="2:36">
-      <c r="B39" s="101"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="16"/>
       <c r="D39" s="2"/>
       <c r="E39" s="27" t="s">
@@ -4534,10 +4509,10 @@
         <v>289600</v>
       </c>
       <c r="AI39" s="20"/>
-      <c r="AJ39" s="100"/>
+      <c r="AJ39" s="98"/>
     </row>
     <row r="40" spans="2:36">
-      <c r="B40" s="101"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="16" t="s">
         <v>12</v>
       </c>
@@ -4583,10 +4558,10 @@
       <c r="AG40" s="2"/>
       <c r="AH40" s="20"/>
       <c r="AI40" s="20"/>
-      <c r="AJ40" s="100"/>
+      <c r="AJ40" s="98"/>
     </row>
     <row r="41" spans="2:36">
-      <c r="B41" s="101"/>
+      <c r="B41" s="99"/>
       <c r="C41" s="16" t="s">
         <v>13</v>
       </c>
@@ -4637,10 +4612,10 @@
       <c r="AG41" s="2"/>
       <c r="AH41" s="20"/>
       <c r="AI41" s="20"/>
-      <c r="AJ41" s="100"/>
+      <c r="AJ41" s="98"/>
     </row>
     <row r="42" spans="2:36">
-      <c r="B42" s="103"/>
+      <c r="B42" s="101"/>
       <c r="C42" s="35" t="s">
         <v>14</v>
       </c>
@@ -4685,10 +4660,10 @@
       <c r="AG42" s="36"/>
       <c r="AH42" s="40"/>
       <c r="AI42" s="40"/>
-      <c r="AJ42" s="106"/>
+      <c r="AJ42" s="104"/>
     </row>
     <row r="43" spans="2:36">
-      <c r="B43" s="101"/>
+      <c r="B43" s="99"/>
       <c r="C43" s="16"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -4722,10 +4697,10 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="20"/>
       <c r="AI43" s="20"/>
-      <c r="AJ43" s="100"/>
+      <c r="AJ43" s="98"/>
     </row>
     <row r="44" spans="2:36">
-      <c r="B44" s="108" t="s">
+      <c r="B44" s="106" t="s">
         <v>28</v>
       </c>
       <c r="C44" s="2"/>
@@ -4761,10 +4736,10 @@
       <c r="AG44" s="2"/>
       <c r="AH44" s="20"/>
       <c r="AI44" s="20"/>
-      <c r="AJ44" s="100"/>
+      <c r="AJ44" s="98"/>
     </row>
     <row r="45" spans="2:36">
-      <c r="B45" s="101"/>
+      <c r="B45" s="99"/>
       <c r="C45" s="16"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -4798,10 +4773,10 @@
       <c r="AG45" s="2"/>
       <c r="AH45" s="20"/>
       <c r="AI45" s="20"/>
-      <c r="AJ45" s="109"/>
+      <c r="AJ45" s="107"/>
     </row>
     <row r="46" spans="2:36">
-      <c r="B46" s="101"/>
+      <c r="B46" s="99"/>
       <c r="C46" s="132" t="s">
         <v>29</v>
       </c>
@@ -4881,10 +4856,10 @@
         <v>72000</v>
       </c>
       <c r="AI46" s="20"/>
-      <c r="AJ46" s="109"/>
+      <c r="AJ46" s="107"/>
     </row>
     <row r="47" spans="2:36">
-      <c r="B47" s="101"/>
+      <c r="B47" s="99"/>
       <c r="C47" s="132"/>
       <c r="D47" s="2"/>
       <c r="E47" s="27" t="s">
@@ -4935,10 +4910,10 @@
         <v>561600</v>
       </c>
       <c r="AI47" s="20"/>
-      <c r="AJ47" s="109"/>
+      <c r="AJ47" s="107"/>
     </row>
     <row r="48" spans="2:36">
-      <c r="B48" s="101"/>
+      <c r="B48" s="99"/>
       <c r="C48" s="49"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -4972,10 +4947,10 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="20"/>
       <c r="AI48" s="20"/>
-      <c r="AJ48" s="109"/>
+      <c r="AJ48" s="107"/>
     </row>
     <row r="49" spans="2:36">
-      <c r="B49" s="101"/>
+      <c r="B49" s="99"/>
       <c r="C49" s="16" t="s">
         <v>12</v>
       </c>
@@ -5021,10 +4996,10 @@
       <c r="AG49" s="2"/>
       <c r="AH49" s="20"/>
       <c r="AI49" s="20"/>
-      <c r="AJ49" s="109"/>
+      <c r="AJ49" s="107"/>
     </row>
     <row r="50" spans="2:36">
-      <c r="B50" s="101"/>
+      <c r="B50" s="99"/>
       <c r="C50" s="16" t="s">
         <v>13</v>
       </c>
@@ -5075,10 +5050,10 @@
       <c r="AG50" s="2"/>
       <c r="AH50" s="20"/>
       <c r="AI50" s="20"/>
-      <c r="AJ50" s="109"/>
+      <c r="AJ50" s="107"/>
     </row>
     <row r="51" spans="2:36">
-      <c r="B51" s="103"/>
+      <c r="B51" s="101"/>
       <c r="C51" s="35" t="s">
         <v>14</v>
       </c>
@@ -5123,10 +5098,10 @@
       <c r="AG51" s="36"/>
       <c r="AH51" s="40"/>
       <c r="AI51" s="40"/>
-      <c r="AJ51" s="110"/>
+      <c r="AJ51" s="108"/>
     </row>
     <row r="52" spans="2:36">
-      <c r="B52" s="101"/>
+      <c r="B52" s="99"/>
       <c r="C52" s="16"/>
       <c r="D52" s="32"/>
       <c r="E52" s="32"/>
@@ -5160,10 +5135,10 @@
       <c r="AG52" s="2"/>
       <c r="AH52" s="20"/>
       <c r="AI52" s="20"/>
-      <c r="AJ52" s="109"/>
+      <c r="AJ52" s="107"/>
     </row>
     <row r="53" spans="2:36">
-      <c r="B53" s="101"/>
+      <c r="B53" s="99"/>
       <c r="C53" s="16" t="s">
         <v>32</v>
       </c>
@@ -5243,10 +5218,10 @@
         <v>44000</v>
       </c>
       <c r="AI53" s="20"/>
-      <c r="AJ53" s="109"/>
+      <c r="AJ53" s="107"/>
     </row>
     <row r="54" spans="2:36">
-      <c r="B54" s="101"/>
+      <c r="B54" s="99"/>
       <c r="C54" s="16" t="s">
         <v>33</v>
       </c>
@@ -5299,10 +5274,10 @@
         <v>561600</v>
       </c>
       <c r="AI54" s="20"/>
-      <c r="AJ54" s="109"/>
+      <c r="AJ54" s="107"/>
     </row>
     <row r="55" spans="2:36">
-      <c r="B55" s="101"/>
+      <c r="B55" s="99"/>
       <c r="C55" s="16"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -5336,10 +5311,10 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="20"/>
       <c r="AI55" s="20"/>
-      <c r="AJ55" s="109"/>
+      <c r="AJ55" s="107"/>
     </row>
     <row r="56" spans="2:36">
-      <c r="B56" s="101"/>
+      <c r="B56" s="99"/>
       <c r="C56" s="16" t="s">
         <v>12</v>
       </c>
@@ -5385,10 +5360,10 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="20"/>
       <c r="AI56" s="20"/>
-      <c r="AJ56" s="109"/>
+      <c r="AJ56" s="107"/>
     </row>
     <row r="57" spans="2:36">
-      <c r="B57" s="101"/>
+      <c r="B57" s="99"/>
       <c r="C57" s="16" t="s">
         <v>13</v>
       </c>
@@ -5439,63 +5414,64 @@
       <c r="AG57" s="32"/>
       <c r="AH57" s="32"/>
       <c r="AI57" s="32"/>
-      <c r="AJ57" s="102"/>
+      <c r="AJ57" s="100"/>
     </row>
     <row r="58" spans="2:36">
-      <c r="B58" s="111"/>
-      <c r="C58" s="112" t="s">
+      <c r="B58" s="109"/>
+      <c r="C58" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="113"/>
-      <c r="E58" s="113"/>
-      <c r="F58" s="114"/>
-      <c r="G58" s="115"/>
-      <c r="H58" s="116"/>
-      <c r="I58" s="113"/>
-      <c r="J58" s="117"/>
-      <c r="K58" s="117"/>
-      <c r="L58" s="113"/>
-      <c r="M58" s="118"/>
-      <c r="N58" s="119">
+      <c r="D58" s="111"/>
+      <c r="E58" s="111"/>
+      <c r="F58" s="112"/>
+      <c r="G58" s="113"/>
+      <c r="H58" s="114"/>
+      <c r="I58" s="111"/>
+      <c r="J58" s="115"/>
+      <c r="K58" s="115"/>
+      <c r="L58" s="111"/>
+      <c r="M58" s="116"/>
+      <c r="N58" s="117">
         <f>N53-H53</f>
         <v>-5.3492484526967282E-3</v>
       </c>
-      <c r="O58" s="113"/>
-      <c r="P58" s="113"/>
-      <c r="Q58" s="113"/>
-      <c r="R58" s="115"/>
-      <c r="S58" s="120"/>
-      <c r="T58" s="119">
+      <c r="O58" s="111"/>
+      <c r="P58" s="111"/>
+      <c r="Q58" s="111"/>
+      <c r="R58" s="113"/>
+      <c r="S58" s="118"/>
+      <c r="T58" s="117">
         <f>T53-N53</f>
         <v>1.0608123439981854E-2</v>
       </c>
-      <c r="U58" s="115"/>
-      <c r="V58" s="115"/>
-      <c r="W58" s="115"/>
-      <c r="X58" s="115"/>
-      <c r="Y58" s="120"/>
-      <c r="Z58" s="119">
+      <c r="U58" s="113"/>
+      <c r="V58" s="113"/>
+      <c r="W58" s="113"/>
+      <c r="X58" s="113"/>
+      <c r="Y58" s="118"/>
+      <c r="Z58" s="117">
         <f>Z53-T53</f>
         <v>6.8790560471976292E-3</v>
       </c>
-      <c r="AA58" s="115"/>
-      <c r="AB58" s="115"/>
-      <c r="AC58" s="115"/>
-      <c r="AD58" s="115"/>
-      <c r="AE58" s="120"/>
-      <c r="AF58" s="116"/>
-      <c r="AG58" s="115"/>
-      <c r="AH58" s="115"/>
-      <c r="AI58" s="115"/>
-      <c r="AJ58" s="121"/>
+      <c r="AA58" s="113"/>
+      <c r="AB58" s="113"/>
+      <c r="AC58" s="113"/>
+      <c r="AD58" s="113"/>
+      <c r="AE58" s="118"/>
+      <c r="AF58" s="114"/>
+      <c r="AG58" s="113"/>
+      <c r="AH58" s="113"/>
+      <c r="AI58" s="113"/>
+      <c r="AJ58" s="119"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="J19:L19"/>
     <mergeCell ref="P19:R19"/>
+    <mergeCell ref="B3:F3"/>
     <mergeCell ref="V19:X19"/>
     <mergeCell ref="AB19:AD19"/>
     <mergeCell ref="AH19:AJ19"/>

</xml_diff>

<commit_message>
reduce width of pie chart in demo_sample.xlsx to avoid exporting 2 charts to a PDF file.
</commit_message>
<xml_diff>
--- a/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
+++ b/zssapp/WebContent/WEB-INF/books/demo_sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="22995" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="22995" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -1080,16 +1080,19 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1099,9 +1102,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,9 +1175,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.7330779054916986"/>
-          <c:y val="0.30801248699271727"/>
-          <c:w val="0.23499361430395913"/>
+          <c:x val="0.69850984680075712"/>
+          <c:y val="0.30801248699271738"/>
+          <c:w val="0.26956168739639835"/>
           <c:h val="0.37044745057232054"/>
         </c:manualLayout>
       </c:layout>
@@ -1197,7 +1197,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1208,13 +1208,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>200026</xdr:colOff>
+      <xdr:colOff>66676</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
@@ -1527,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2415,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AJ58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2499,55 +2499,55 @@
       <c r="AJ2" s="3"/>
     </row>
     <row r="3" spans="2:36">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="129" t="s">
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="129" t="s">
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="130"/>
-      <c r="O3" s="130"/>
-      <c r="P3" s="130" t="s">
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="130"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="129" t="s">
+      <c r="Q3" s="131"/>
+      <c r="R3" s="131"/>
+      <c r="S3" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="130"/>
-      <c r="U3" s="130"/>
-      <c r="V3" s="130"/>
-      <c r="W3" s="130"/>
-      <c r="X3" s="130"/>
-      <c r="Y3" s="129" t="s">
+      <c r="T3" s="131"/>
+      <c r="U3" s="131"/>
+      <c r="V3" s="131"/>
+      <c r="W3" s="131"/>
+      <c r="X3" s="131"/>
+      <c r="Y3" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="130"/>
-      <c r="AA3" s="130"/>
-      <c r="AB3" s="130"/>
-      <c r="AC3" s="130"/>
-      <c r="AD3" s="130"/>
-      <c r="AE3" s="129" t="s">
+      <c r="Z3" s="131"/>
+      <c r="AA3" s="131"/>
+      <c r="AB3" s="131"/>
+      <c r="AC3" s="131"/>
+      <c r="AD3" s="131"/>
+      <c r="AE3" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="130"/>
-      <c r="AG3" s="130"/>
-      <c r="AH3" s="130"/>
-      <c r="AI3" s="130"/>
-      <c r="AJ3" s="131"/>
+      <c r="AF3" s="131"/>
+      <c r="AG3" s="131"/>
+      <c r="AH3" s="131"/>
+      <c r="AI3" s="131"/>
+      <c r="AJ3" s="132"/>
     </row>
     <row r="4" spans="2:36">
       <c r="B4" s="95" t="s">
@@ -3069,48 +3069,48 @@
       <c r="G13" s="18"/>
       <c r="H13" s="19"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="126">
+      <c r="J13" s="125">
         <f>Input!F20</f>
         <v>23000</v>
       </c>
-      <c r="K13" s="127"/>
-      <c r="L13" s="127"/>
+      <c r="K13" s="126"/>
+      <c r="L13" s="126"/>
       <c r="M13" s="48"/>
       <c r="N13" s="19"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="126">
+      <c r="P13" s="125">
         <f>Input!G20</f>
         <v>25000</v>
       </c>
-      <c r="Q13" s="127"/>
-      <c r="R13" s="127"/>
+      <c r="Q13" s="126"/>
+      <c r="R13" s="126"/>
       <c r="S13" s="48"/>
       <c r="T13" s="19"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="126">
+      <c r="V13" s="125">
         <f>Input!H20</f>
         <v>22500</v>
       </c>
-      <c r="W13" s="127"/>
-      <c r="X13" s="127"/>
+      <c r="W13" s="126"/>
+      <c r="X13" s="126"/>
       <c r="Y13" s="48"/>
       <c r="Z13" s="19"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="126">
+      <c r="AB13" s="125">
         <f>Input!I20</f>
         <v>25600</v>
       </c>
-      <c r="AC13" s="127"/>
-      <c r="AD13" s="127"/>
+      <c r="AC13" s="126"/>
+      <c r="AD13" s="126"/>
       <c r="AE13" s="48"/>
       <c r="AF13" s="19"/>
       <c r="AG13" s="2"/>
-      <c r="AH13" s="126">
+      <c r="AH13" s="125">
         <f>Input!J20</f>
         <v>96100</v>
       </c>
-      <c r="AI13" s="127"/>
-      <c r="AJ13" s="128"/>
+      <c r="AI13" s="126"/>
+      <c r="AJ13" s="129"/>
     </row>
     <row r="14" spans="2:36">
       <c r="B14" s="99"/>
@@ -3302,7 +3302,7 @@
     </row>
     <row r="18" spans="2:36">
       <c r="B18" s="99"/>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="124" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -3410,7 +3410,7 @@
     </row>
     <row r="19" spans="2:36">
       <c r="B19" s="99"/>
-      <c r="C19" s="132"/>
+      <c r="C19" s="124"/>
       <c r="D19" s="2"/>
       <c r="E19" s="27" t="s">
         <v>20</v>
@@ -3419,48 +3419,48 @@
       <c r="G19" s="18"/>
       <c r="H19" s="19"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="126">
+      <c r="J19" s="125">
         <f>Input!F15</f>
         <v>125000</v>
       </c>
-      <c r="K19" s="127"/>
-      <c r="L19" s="127"/>
+      <c r="K19" s="126"/>
+      <c r="L19" s="126"/>
       <c r="M19" s="48"/>
       <c r="N19" s="19"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="126">
+      <c r="P19" s="125">
         <f>Input!G15</f>
         <v>126000</v>
       </c>
-      <c r="Q19" s="127"/>
-      <c r="R19" s="127"/>
+      <c r="Q19" s="126"/>
+      <c r="R19" s="126"/>
       <c r="S19" s="48"/>
       <c r="T19" s="19"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="126">
+      <c r="V19" s="125">
         <f>Input!H15</f>
         <v>126500</v>
       </c>
-      <c r="W19" s="127"/>
-      <c r="X19" s="127"/>
+      <c r="W19" s="126"/>
+      <c r="X19" s="126"/>
       <c r="Y19" s="48"/>
       <c r="Z19" s="19"/>
       <c r="AA19" s="2"/>
-      <c r="AB19" s="126">
+      <c r="AB19" s="125">
         <f>Input!I15</f>
         <v>136000</v>
       </c>
-      <c r="AC19" s="127"/>
-      <c r="AD19" s="127"/>
+      <c r="AC19" s="126"/>
+      <c r="AD19" s="126"/>
       <c r="AE19" s="48"/>
       <c r="AF19" s="25"/>
       <c r="AG19" s="2"/>
-      <c r="AH19" s="126">
+      <c r="AH19" s="125">
         <f>Input!J15</f>
         <v>513500</v>
       </c>
-      <c r="AI19" s="127"/>
-      <c r="AJ19" s="128"/>
+      <c r="AI19" s="126"/>
+      <c r="AJ19" s="129"/>
     </row>
     <row r="20" spans="2:36">
       <c r="B20" s="99"/>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="25" spans="2:36">
       <c r="B25" s="99"/>
-      <c r="C25" s="132" t="s">
+      <c r="C25" s="124" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -3772,7 +3772,7 @@
     </row>
     <row r="26" spans="2:36">
       <c r="B26" s="99"/>
-      <c r="C26" s="132"/>
+      <c r="C26" s="124"/>
       <c r="D26" s="2"/>
       <c r="E26" s="27" t="s">
         <v>22</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="46" spans="2:36">
       <c r="B46" s="99"/>
-      <c r="C46" s="132" t="s">
+      <c r="C46" s="124" t="s">
         <v>29</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -4860,7 +4860,7 @@
     </row>
     <row r="47" spans="2:36">
       <c r="B47" s="99"/>
-      <c r="C47" s="132"/>
+      <c r="C47" s="124"/>
       <c r="D47" s="2"/>
       <c r="E47" s="27" t="s">
         <v>31</v>
@@ -5466,11 +5466,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="P19:R19"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="V19:X19"/>
     <mergeCell ref="AB19:AD19"/>
@@ -5485,6 +5480,11 @@
     <mergeCell ref="V13:X13"/>
     <mergeCell ref="AB13:AD13"/>
     <mergeCell ref="AH13:AJ13"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="P19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>